<commit_message>
Improved RK indiv programs
</commit_message>
<xml_diff>
--- a/CompLaagBond/files/template-excel-bk-25m1pijl-teams.xlsx
+++ b/CompLaagBond/files/template-excel-bk-25m1pijl-teams.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects Ramon\Websites\NHB-applicaties\Excel programma's\BK excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40C9682-863A-4C03-A71D-41349281E41E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F1DD42-32BC-44FB-9857-5306BB2D7B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5700" yWindow="1065" windowWidth="22440" windowHeight="14040" tabRatio="546" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2595" yWindow="810" windowWidth="22440" windowHeight="14040" tabRatio="546" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Uitleg" sheetId="16" r:id="rId1"/>
@@ -548,6 +548,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1455,35 +1456,8 @@
     <xf numFmtId="1" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -1495,28 +1469,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="43" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="42" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1534,22 +1491,19 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="43" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="43" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1568,22 +1522,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="1" fontId="7" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1604,13 +1543,7 @@
     <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1621,19 +1554,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1742,6 +1666,83 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="45" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="45" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2200,10 +2201,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:2" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="61" t="s">
+      <c r="A4" s="138" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="61"/>
+      <c r="B4" s="138"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
@@ -2378,17 +2379,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="24" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="62" t="str">
+      <c r="B1" s="139" t="str">
         <f>'Deelnemers en Scores'!B2</f>
         <v>BK 25m1pijl Teams, Klasse: komt hier</v>
       </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="64"/>
+      <c r="C1" s="140"/>
+      <c r="D1" s="140"/>
+      <c r="E1" s="140"/>
+      <c r="F1" s="140"/>
+      <c r="G1" s="140"/>
+      <c r="H1" s="140"/>
+      <c r="I1" s="141"/>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C2" s="10"/>
@@ -2400,7 +2401,7 @@
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4" s="3"/>
-      <c r="C4" s="65"/>
+      <c r="C4" s="61"/>
       <c r="D4" s="3"/>
       <c r="G4" s="36"/>
       <c r="H4" s="36"/>
@@ -2533,168 +2534,168 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.109375" style="71" customWidth="1"/>
-    <col min="2" max="2" width="4.44140625" style="139" customWidth="1"/>
-    <col min="3" max="3" width="5.109375" style="139" customWidth="1"/>
-    <col min="4" max="4" width="29.33203125" style="139" customWidth="1"/>
-    <col min="5" max="5" width="7.77734375" style="71" customWidth="1"/>
-    <col min="6" max="6" width="34.44140625" style="71" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" style="72" customWidth="1"/>
-    <col min="8" max="9" width="3.6640625" style="73" customWidth="1"/>
-    <col min="10" max="10" width="6.77734375" style="73" customWidth="1"/>
-    <col min="11" max="11" width="6.77734375" style="71" customWidth="1"/>
-    <col min="12" max="12" width="2.21875" style="71" customWidth="1"/>
-    <col min="13" max="16384" width="7.109375" style="71" hidden="1"/>
+    <col min="1" max="1" width="3.109375" style="64" customWidth="1"/>
+    <col min="2" max="2" width="4.44140625" style="117" customWidth="1"/>
+    <col min="3" max="3" width="5.109375" style="117" customWidth="1"/>
+    <col min="4" max="4" width="29.33203125" style="117" customWidth="1"/>
+    <col min="5" max="5" width="7.77734375" style="64" customWidth="1"/>
+    <col min="6" max="6" width="34.44140625" style="64" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" style="65" customWidth="1"/>
+    <col min="8" max="9" width="3.6640625" style="66" customWidth="1"/>
+    <col min="10" max="10" width="6.77734375" style="66" customWidth="1"/>
+    <col min="11" max="11" width="6.77734375" style="64" customWidth="1"/>
+    <col min="12" max="12" width="2.21875" style="64" customWidth="1"/>
+    <col min="13" max="16384" width="7.109375" style="64" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:11" ht="24" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="142" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="68"/>
+      <c r="C2" s="143"/>
+      <c r="D2" s="143"/>
+      <c r="E2" s="143"/>
+      <c r="F2" s="143"/>
+      <c r="G2" s="143"/>
+      <c r="H2" s="143"/>
+      <c r="I2" s="143"/>
+      <c r="J2" s="143"/>
+      <c r="K2" s="144"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B3" s="69"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="K3" s="74"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="K3" s="67"/>
     </row>
     <row r="4" spans="2:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="75" t="s">
+      <c r="B4" s="146" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="77" t="s">
+      <c r="C4" s="147"/>
+      <c r="D4" s="147"/>
+      <c r="E4" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="78" t="s">
+      <c r="F4" s="148" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="79" t="s">
+      <c r="G4" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="80" t="s">
+      <c r="H4" s="149" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="80"/>
-      <c r="J4" s="80"/>
-      <c r="K4" s="81"/>
+      <c r="I4" s="149"/>
+      <c r="J4" s="149"/>
+      <c r="K4" s="150"/>
     </row>
     <row r="5" spans="2:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="B5" s="82"/>
-      <c r="C5" s="83"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="83"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="83"/>
-      <c r="H5" s="85"/>
-      <c r="I5" s="85"/>
-      <c r="J5" s="85"/>
-      <c r="K5" s="86"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="148"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="73"/>
+      <c r="K5" s="74"/>
     </row>
     <row r="6" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="94"/>
-      <c r="C6" s="87"/>
-      <c r="D6" s="87"/>
-      <c r="E6" s="87"/>
-      <c r="F6" s="88" t="s">
+      <c r="B6" s="81"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="89" t="s">
+      <c r="G6" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="H6" s="90" t="s">
+      <c r="H6" s="145" t="s">
         <v>48</v>
       </c>
-      <c r="I6" s="90"/>
-      <c r="J6" s="87" t="s">
+      <c r="I6" s="145"/>
+      <c r="J6" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="K6" s="93" t="s">
+      <c r="K6" s="80" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B7" s="94" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="87" t="s">
+      <c r="B7" s="81" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="88" t="s">
+      <c r="D7" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="87" t="s">
+      <c r="E7" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="88" t="s">
+      <c r="F7" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="91" t="s">
+      <c r="G7" s="78" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="92" t="s">
+      <c r="H7" s="79" t="s">
         <v>49</v>
       </c>
-      <c r="I7" s="92" t="s">
+      <c r="I7" s="79" t="s">
         <v>50</v>
       </c>
-      <c r="J7" s="87" t="s">
+      <c r="J7" s="75" t="s">
         <v>39</v>
       </c>
-      <c r="K7" s="93" t="s">
+      <c r="K7" s="80" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B8" s="138"/>
-      <c r="E8" s="139"/>
-      <c r="F8" s="139"/>
-      <c r="G8" s="140"/>
-      <c r="H8" s="139"/>
-      <c r="I8" s="139"/>
-      <c r="J8" s="139"/>
-      <c r="K8" s="141"/>
+      <c r="B8" s="116"/>
+      <c r="E8" s="117"/>
+      <c r="F8" s="117"/>
+      <c r="G8" s="118"/>
+      <c r="H8" s="117"/>
+      <c r="I8" s="117"/>
+      <c r="J8" s="117"/>
+      <c r="K8" s="119"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B9" s="142">
+      <c r="B9" s="120">
         <v>1</v>
       </c>
-      <c r="C9" s="143">
+      <c r="C9" s="121">
         <v>100</v>
       </c>
-      <c r="D9" s="144" t="s">
+      <c r="D9" s="122" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="143"/>
-      <c r="F9" s="144" t="s">
+      <c r="E9" s="121"/>
+      <c r="F9" s="122" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="145">
+      <c r="G9" s="123">
         <v>888.8</v>
       </c>
-      <c r="H9" s="143"/>
-      <c r="I9" s="143"/>
-      <c r="J9" s="139"/>
-      <c r="K9" s="146">
+      <c r="H9" s="121"/>
+      <c r="I9" s="121"/>
+      <c r="J9" s="117"/>
+      <c r="K9" s="124">
         <f>IF(COUNTA(J10:J13)&lt;3,0,IF(COUNTA(J10:J13)=3,SUM(J10:J13),IF(SUM(J10:J13)&gt;0,SUM(J10:J13)-MINA(J10:J13),0)))</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="142"/>
-      <c r="C10" s="143"/>
-      <c r="D10" s="143"/>
+      <c r="B10" s="120"/>
+      <c r="C10" s="121"/>
+      <c r="D10" s="121"/>
       <c r="E10" s="8">
         <v>123456</v>
       </c>
@@ -2710,16 +2711,16 @@
       <c r="I10" s="8">
         <v>0</v>
       </c>
-      <c r="J10" s="73">
+      <c r="J10" s="66">
         <f>SUM(H10:I10)</f>
         <v>0</v>
       </c>
-      <c r="K10" s="74"/>
+      <c r="K10" s="67"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B11" s="142"/>
-      <c r="C11" s="143"/>
-      <c r="D11" s="143"/>
+      <c r="B11" s="120"/>
+      <c r="C11" s="121"/>
+      <c r="D11" s="121"/>
       <c r="E11" s="8">
         <v>123456</v>
       </c>
@@ -2735,16 +2736,16 @@
       <c r="I11" s="8">
         <v>0</v>
       </c>
-      <c r="J11" s="73">
+      <c r="J11" s="66">
         <f>SUM(H11:I11)</f>
         <v>0</v>
       </c>
-      <c r="K11" s="74"/>
+      <c r="K11" s="67"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B12" s="142"/>
-      <c r="C12" s="143"/>
-      <c r="D12" s="143"/>
+      <c r="B12" s="120"/>
+      <c r="C12" s="121"/>
+      <c r="D12" s="121"/>
       <c r="E12" s="8">
         <v>123456</v>
       </c>
@@ -2760,16 +2761,16 @@
       <c r="I12" s="8">
         <v>0</v>
       </c>
-      <c r="J12" s="73">
+      <c r="J12" s="66">
         <f>SUM(H12:I12)</f>
         <v>0</v>
       </c>
-      <c r="K12" s="74"/>
+      <c r="K12" s="67"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B13" s="142"/>
-      <c r="C13" s="143"/>
-      <c r="D13" s="143"/>
+      <c r="B13" s="120"/>
+      <c r="C13" s="121"/>
+      <c r="D13" s="121"/>
       <c r="E13" s="8">
         <v>123456</v>
       </c>
@@ -2785,52 +2786,52 @@
       <c r="I13" s="8">
         <v>0</v>
       </c>
-      <c r="J13" s="73">
+      <c r="J13" s="66">
         <f>SUM(H13:I13)</f>
         <v>0</v>
       </c>
-      <c r="K13" s="74"/>
+      <c r="K13" s="67"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B14" s="142"/>
-      <c r="C14" s="143"/>
-      <c r="D14" s="143"/>
-      <c r="E14" s="148"/>
-      <c r="F14" s="152"/>
-      <c r="G14" s="153"/>
-      <c r="H14" s="148"/>
-      <c r="I14" s="148"/>
-      <c r="K14" s="74"/>
+      <c r="B14" s="120"/>
+      <c r="C14" s="121"/>
+      <c r="D14" s="121"/>
+      <c r="E14" s="126"/>
+      <c r="F14" s="130"/>
+      <c r="G14" s="131"/>
+      <c r="H14" s="126"/>
+      <c r="I14" s="126"/>
+      <c r="K14" s="67"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B15" s="142">
+      <c r="B15" s="120">
         <v>2</v>
       </c>
-      <c r="C15" s="143">
+      <c r="C15" s="121">
         <v>100</v>
       </c>
-      <c r="D15" s="144" t="s">
+      <c r="D15" s="122" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="143"/>
-      <c r="F15" s="144" t="s">
+      <c r="E15" s="121"/>
+      <c r="F15" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="145">
+      <c r="G15" s="123">
         <v>888.8</v>
       </c>
-      <c r="H15" s="148"/>
-      <c r="I15" s="148"/>
-      <c r="J15" s="139"/>
-      <c r="K15" s="146">
+      <c r="H15" s="126"/>
+      <c r="I15" s="126"/>
+      <c r="J15" s="117"/>
+      <c r="K15" s="124">
         <f>IF(COUNTA(J16:J19)&lt;3,0,IF(COUNTA(J16:J19)=3,SUM(J16:J19),IF(SUM(J16:J19)&gt;0,SUM(J16:J19)-MINA(J16:J19),0)))</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B16" s="142"/>
-      <c r="C16" s="143"/>
-      <c r="D16" s="143"/>
+      <c r="B16" s="120"/>
+      <c r="C16" s="121"/>
+      <c r="D16" s="121"/>
       <c r="E16" s="8">
         <v>123456</v>
       </c>
@@ -2846,16 +2847,16 @@
       <c r="I16" s="8">
         <v>0</v>
       </c>
-      <c r="J16" s="73">
+      <c r="J16" s="66">
         <f>SUM(H16:I16)</f>
         <v>0</v>
       </c>
-      <c r="K16" s="74"/>
+      <c r="K16" s="67"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B17" s="142"/>
-      <c r="C17" s="143"/>
-      <c r="D17" s="143"/>
+      <c r="B17" s="120"/>
+      <c r="C17" s="121"/>
+      <c r="D17" s="121"/>
       <c r="E17" s="8">
         <v>123456</v>
       </c>
@@ -2871,16 +2872,16 @@
       <c r="I17" s="8">
         <v>0</v>
       </c>
-      <c r="J17" s="73">
+      <c r="J17" s="66">
         <f>SUM(H17:I17)</f>
         <v>0</v>
       </c>
-      <c r="K17" s="74"/>
+      <c r="K17" s="67"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B18" s="142"/>
-      <c r="C18" s="143"/>
-      <c r="D18" s="143"/>
+      <c r="B18" s="120"/>
+      <c r="C18" s="121"/>
+      <c r="D18" s="121"/>
       <c r="E18" s="8">
         <v>123456</v>
       </c>
@@ -2896,16 +2897,16 @@
       <c r="I18" s="8">
         <v>0</v>
       </c>
-      <c r="J18" s="73">
+      <c r="J18" s="66">
         <f>SUM(H18:I18)</f>
         <v>0</v>
       </c>
-      <c r="K18" s="74"/>
+      <c r="K18" s="67"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B19" s="142"/>
-      <c r="C19" s="143"/>
-      <c r="D19" s="143"/>
+      <c r="B19" s="120"/>
+      <c r="C19" s="121"/>
+      <c r="D19" s="121"/>
       <c r="E19" s="8">
         <v>123456</v>
       </c>
@@ -2921,52 +2922,52 @@
       <c r="I19" s="8">
         <v>0</v>
       </c>
-      <c r="J19" s="73">
+      <c r="J19" s="66">
         <f>SUM(H19:I19)</f>
         <v>0</v>
       </c>
-      <c r="K19" s="74"/>
+      <c r="K19" s="67"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B20" s="142"/>
-      <c r="C20" s="143"/>
-      <c r="D20" s="143"/>
-      <c r="E20" s="148"/>
-      <c r="F20" s="152"/>
-      <c r="G20" s="153"/>
-      <c r="H20" s="148"/>
-      <c r="I20" s="148"/>
-      <c r="K20" s="74"/>
+      <c r="B20" s="120"/>
+      <c r="C20" s="121"/>
+      <c r="D20" s="121"/>
+      <c r="E20" s="126"/>
+      <c r="F20" s="130"/>
+      <c r="G20" s="131"/>
+      <c r="H20" s="126"/>
+      <c r="I20" s="126"/>
+      <c r="K20" s="67"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B21" s="142">
+      <c r="B21" s="120">
         <v>3</v>
       </c>
-      <c r="C21" s="143">
+      <c r="C21" s="121">
         <v>100</v>
       </c>
-      <c r="D21" s="144" t="s">
+      <c r="D21" s="122" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="143"/>
-      <c r="F21" s="144" t="s">
+      <c r="E21" s="121"/>
+      <c r="F21" s="122" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="145">
+      <c r="G21" s="123">
         <v>888.8</v>
       </c>
-      <c r="H21" s="148"/>
-      <c r="I21" s="148"/>
-      <c r="J21" s="139"/>
-      <c r="K21" s="146">
+      <c r="H21" s="126"/>
+      <c r="I21" s="126"/>
+      <c r="J21" s="117"/>
+      <c r="K21" s="124">
         <f>IF(COUNTA(J22:J25)&lt;3,0,IF(COUNTA(J22:J25)=3,SUM(J22:J25),IF(SUM(J22:J25)&gt;0,SUM(J22:J25)-MINA(J22:J25),0)))</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B22" s="142"/>
-      <c r="C22" s="143"/>
-      <c r="D22" s="143"/>
+      <c r="B22" s="120"/>
+      <c r="C22" s="121"/>
+      <c r="D22" s="121"/>
       <c r="E22" s="8">
         <v>123456</v>
       </c>
@@ -2982,16 +2983,16 @@
       <c r="I22" s="8">
         <v>0</v>
       </c>
-      <c r="J22" s="73">
+      <c r="J22" s="66">
         <f>SUM(H22:I22)</f>
         <v>0</v>
       </c>
-      <c r="K22" s="74"/>
+      <c r="K22" s="67"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B23" s="142"/>
-      <c r="C23" s="143"/>
-      <c r="D23" s="143"/>
+      <c r="B23" s="120"/>
+      <c r="C23" s="121"/>
+      <c r="D23" s="121"/>
       <c r="E23" s="8">
         <v>123456</v>
       </c>
@@ -3007,16 +3008,16 @@
       <c r="I23" s="8">
         <v>0</v>
       </c>
-      <c r="J23" s="73">
+      <c r="J23" s="66">
         <f>SUM(H23:I23)</f>
         <v>0</v>
       </c>
-      <c r="K23" s="74"/>
+      <c r="K23" s="67"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B24" s="142"/>
-      <c r="C24" s="143"/>
-      <c r="D24" s="143"/>
+      <c r="B24" s="120"/>
+      <c r="C24" s="121"/>
+      <c r="D24" s="121"/>
       <c r="E24" s="8">
         <v>123456</v>
       </c>
@@ -3032,16 +3033,16 @@
       <c r="I24" s="8">
         <v>0</v>
       </c>
-      <c r="J24" s="73">
+      <c r="J24" s="66">
         <f>SUM(H24:I24)</f>
         <v>0</v>
       </c>
-      <c r="K24" s="74"/>
+      <c r="K24" s="67"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B25" s="142"/>
-      <c r="C25" s="143"/>
-      <c r="D25" s="143"/>
+      <c r="B25" s="120"/>
+      <c r="C25" s="121"/>
+      <c r="D25" s="121"/>
       <c r="E25" s="8">
         <v>123456</v>
       </c>
@@ -3057,52 +3058,52 @@
       <c r="I25" s="8">
         <v>0</v>
       </c>
-      <c r="J25" s="73">
+      <c r="J25" s="66">
         <f>SUM(H25:I25)</f>
         <v>0</v>
       </c>
-      <c r="K25" s="74"/>
+      <c r="K25" s="67"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B26" s="142"/>
-      <c r="C26" s="143"/>
-      <c r="D26" s="143"/>
-      <c r="E26" s="148"/>
-      <c r="F26" s="152"/>
-      <c r="G26" s="153"/>
-      <c r="H26" s="148"/>
-      <c r="I26" s="148"/>
-      <c r="K26" s="74"/>
+      <c r="B26" s="120"/>
+      <c r="C26" s="121"/>
+      <c r="D26" s="121"/>
+      <c r="E26" s="126"/>
+      <c r="F26" s="130"/>
+      <c r="G26" s="131"/>
+      <c r="H26" s="126"/>
+      <c r="I26" s="126"/>
+      <c r="K26" s="67"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B27" s="142">
+      <c r="B27" s="120">
         <v>4</v>
       </c>
-      <c r="C27" s="143">
+      <c r="C27" s="121">
         <v>100</v>
       </c>
-      <c r="D27" s="144" t="s">
+      <c r="D27" s="122" t="s">
         <v>31</v>
       </c>
-      <c r="E27" s="143"/>
-      <c r="F27" s="144" t="s">
+      <c r="E27" s="121"/>
+      <c r="F27" s="122" t="s">
         <v>16</v>
       </c>
-      <c r="G27" s="145">
+      <c r="G27" s="123">
         <v>888.8</v>
       </c>
-      <c r="H27" s="148"/>
-      <c r="I27" s="148"/>
-      <c r="J27" s="139"/>
-      <c r="K27" s="146">
+      <c r="H27" s="126"/>
+      <c r="I27" s="126"/>
+      <c r="J27" s="117"/>
+      <c r="K27" s="124">
         <f>IF(COUNTA(J28:J31)&lt;3,0,IF(COUNTA(J28:J31)=3,SUM(J28:J31),IF(SUM(J28:J31)&gt;0,SUM(J28:J31)-MINA(J28:J31),0)))</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B28" s="142"/>
-      <c r="C28" s="143"/>
-      <c r="D28" s="143"/>
+      <c r="B28" s="120"/>
+      <c r="C28" s="121"/>
+      <c r="D28" s="121"/>
       <c r="E28" s="8">
         <v>123456</v>
       </c>
@@ -3118,16 +3119,16 @@
       <c r="I28" s="8">
         <v>0</v>
       </c>
-      <c r="J28" s="73">
+      <c r="J28" s="66">
         <f>SUM(H28:I28)</f>
         <v>0</v>
       </c>
-      <c r="K28" s="74"/>
+      <c r="K28" s="67"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B29" s="142"/>
-      <c r="C29" s="143"/>
-      <c r="D29" s="143"/>
+      <c r="B29" s="120"/>
+      <c r="C29" s="121"/>
+      <c r="D29" s="121"/>
       <c r="E29" s="8">
         <v>123456</v>
       </c>
@@ -3143,16 +3144,16 @@
       <c r="I29" s="8">
         <v>0</v>
       </c>
-      <c r="J29" s="73">
+      <c r="J29" s="66">
         <f>SUM(H29:I29)</f>
         <v>0</v>
       </c>
-      <c r="K29" s="74"/>
+      <c r="K29" s="67"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B30" s="142"/>
-      <c r="C30" s="143"/>
-      <c r="D30" s="143"/>
+      <c r="B30" s="120"/>
+      <c r="C30" s="121"/>
+      <c r="D30" s="121"/>
       <c r="E30" s="8">
         <v>123456</v>
       </c>
@@ -3168,16 +3169,16 @@
       <c r="I30" s="8">
         <v>0</v>
       </c>
-      <c r="J30" s="73">
+      <c r="J30" s="66">
         <f>SUM(H30:I30)</f>
         <v>0</v>
       </c>
-      <c r="K30" s="74"/>
+      <c r="K30" s="67"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B31" s="142"/>
-      <c r="C31" s="143"/>
-      <c r="D31" s="143"/>
+      <c r="B31" s="120"/>
+      <c r="C31" s="121"/>
+      <c r="D31" s="121"/>
       <c r="E31" s="8">
         <v>123456</v>
       </c>
@@ -3193,52 +3194,52 @@
       <c r="I31" s="8">
         <v>0</v>
       </c>
-      <c r="J31" s="73">
+      <c r="J31" s="66">
         <f>SUM(H31:I31)</f>
         <v>0</v>
       </c>
-      <c r="K31" s="74"/>
+      <c r="K31" s="67"/>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B32" s="142"/>
-      <c r="C32" s="143"/>
-      <c r="D32" s="143"/>
-      <c r="E32" s="148"/>
-      <c r="F32" s="152"/>
-      <c r="G32" s="153"/>
-      <c r="H32" s="148"/>
-      <c r="I32" s="148"/>
-      <c r="K32" s="74"/>
+      <c r="B32" s="120"/>
+      <c r="C32" s="121"/>
+      <c r="D32" s="121"/>
+      <c r="E32" s="126"/>
+      <c r="F32" s="130"/>
+      <c r="G32" s="131"/>
+      <c r="H32" s="126"/>
+      <c r="I32" s="126"/>
+      <c r="K32" s="67"/>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B33" s="142">
+      <c r="B33" s="120">
         <v>5</v>
       </c>
-      <c r="C33" s="143">
+      <c r="C33" s="121">
         <v>100</v>
       </c>
-      <c r="D33" s="144" t="s">
+      <c r="D33" s="122" t="s">
         <v>32</v>
       </c>
-      <c r="E33" s="143"/>
-      <c r="F33" s="144" t="s">
+      <c r="E33" s="121"/>
+      <c r="F33" s="122" t="s">
         <v>33</v>
       </c>
-      <c r="G33" s="145">
+      <c r="G33" s="123">
         <v>888.8</v>
       </c>
-      <c r="H33" s="148"/>
-      <c r="I33" s="148"/>
-      <c r="J33" s="139"/>
-      <c r="K33" s="146">
+      <c r="H33" s="126"/>
+      <c r="I33" s="126"/>
+      <c r="J33" s="117"/>
+      <c r="K33" s="124">
         <f>IF(COUNTA(J34:J37)&lt;3,0,IF(COUNTA(J34:J37)=3,SUM(J34:J37),IF(SUM(J34:J37)&gt;0,SUM(J34:J37)-MINA(J34:J37),0)))</f>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B34" s="142"/>
-      <c r="C34" s="143"/>
-      <c r="D34" s="143"/>
+      <c r="B34" s="120"/>
+      <c r="C34" s="121"/>
+      <c r="D34" s="121"/>
       <c r="E34" s="8">
         <v>123456</v>
       </c>
@@ -3254,16 +3255,16 @@
       <c r="I34" s="8">
         <v>0</v>
       </c>
-      <c r="J34" s="73">
+      <c r="J34" s="66">
         <f>SUM(H34:I34)</f>
         <v>0</v>
       </c>
-      <c r="K34" s="74"/>
+      <c r="K34" s="67"/>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B35" s="142"/>
-      <c r="C35" s="143"/>
-      <c r="D35" s="143"/>
+      <c r="B35" s="120"/>
+      <c r="C35" s="121"/>
+      <c r="D35" s="121"/>
       <c r="E35" s="8">
         <v>123456</v>
       </c>
@@ -3279,16 +3280,16 @@
       <c r="I35" s="8">
         <v>0</v>
       </c>
-      <c r="J35" s="73">
+      <c r="J35" s="66">
         <f>SUM(H35:I35)</f>
         <v>0</v>
       </c>
-      <c r="K35" s="74"/>
+      <c r="K35" s="67"/>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B36" s="142"/>
-      <c r="C36" s="143"/>
-      <c r="D36" s="143"/>
+      <c r="B36" s="120"/>
+      <c r="C36" s="121"/>
+      <c r="D36" s="121"/>
       <c r="E36" s="8">
         <v>123456</v>
       </c>
@@ -3304,16 +3305,16 @@
       <c r="I36" s="8">
         <v>0</v>
       </c>
-      <c r="J36" s="73">
+      <c r="J36" s="66">
         <f>SUM(H36:I36)</f>
         <v>0</v>
       </c>
-      <c r="K36" s="74"/>
+      <c r="K36" s="67"/>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B37" s="142"/>
-      <c r="C37" s="143"/>
-      <c r="D37" s="143"/>
+      <c r="B37" s="120"/>
+      <c r="C37" s="121"/>
+      <c r="D37" s="121"/>
       <c r="E37" s="8">
         <v>123456</v>
       </c>
@@ -3329,52 +3330,52 @@
       <c r="I37" s="8">
         <v>0</v>
       </c>
-      <c r="J37" s="73">
+      <c r="J37" s="66">
         <f>SUM(H37:I37)</f>
         <v>0</v>
       </c>
-      <c r="K37" s="74"/>
+      <c r="K37" s="67"/>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B38" s="142"/>
-      <c r="C38" s="143"/>
-      <c r="D38" s="143"/>
-      <c r="E38" s="148"/>
-      <c r="F38" s="152"/>
-      <c r="G38" s="153"/>
-      <c r="H38" s="148"/>
-      <c r="I38" s="148"/>
-      <c r="K38" s="74"/>
+      <c r="B38" s="120"/>
+      <c r="C38" s="121"/>
+      <c r="D38" s="121"/>
+      <c r="E38" s="126"/>
+      <c r="F38" s="130"/>
+      <c r="G38" s="131"/>
+      <c r="H38" s="126"/>
+      <c r="I38" s="126"/>
+      <c r="K38" s="67"/>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B39" s="142">
+      <c r="B39" s="120">
         <v>6</v>
       </c>
-      <c r="C39" s="143">
+      <c r="C39" s="121">
         <v>100</v>
       </c>
-      <c r="D39" s="144" t="s">
+      <c r="D39" s="122" t="s">
         <v>29</v>
       </c>
-      <c r="E39" s="143"/>
-      <c r="F39" s="144" t="s">
+      <c r="E39" s="121"/>
+      <c r="F39" s="122" t="s">
         <v>30</v>
       </c>
-      <c r="G39" s="145">
+      <c r="G39" s="123">
         <v>888.8</v>
       </c>
-      <c r="H39" s="148"/>
-      <c r="I39" s="148"/>
-      <c r="J39" s="139"/>
-      <c r="K39" s="146">
+      <c r="H39" s="126"/>
+      <c r="I39" s="126"/>
+      <c r="J39" s="117"/>
+      <c r="K39" s="124">
         <f>IF(COUNTA(J40:J43)&lt;3,0,IF(COUNTA(J40:J43)=3,SUM(J40:J43),IF(SUM(J40:J43)&gt;0,SUM(J40:J43)-MINA(J40:J43),0)))</f>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B40" s="142"/>
-      <c r="C40" s="143"/>
-      <c r="D40" s="143"/>
+      <c r="B40" s="120"/>
+      <c r="C40" s="121"/>
+      <c r="D40" s="121"/>
       <c r="E40" s="8">
         <v>123456</v>
       </c>
@@ -3390,16 +3391,16 @@
       <c r="I40" s="8">
         <v>0</v>
       </c>
-      <c r="J40" s="73">
+      <c r="J40" s="66">
         <f>SUM(H40:I40)</f>
         <v>0</v>
       </c>
-      <c r="K40" s="74"/>
+      <c r="K40" s="67"/>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B41" s="142"/>
-      <c r="C41" s="143"/>
-      <c r="D41" s="143"/>
+      <c r="B41" s="120"/>
+      <c r="C41" s="121"/>
+      <c r="D41" s="121"/>
       <c r="E41" s="8">
         <v>123456</v>
       </c>
@@ -3415,16 +3416,16 @@
       <c r="I41" s="8">
         <v>0</v>
       </c>
-      <c r="J41" s="73">
+      <c r="J41" s="66">
         <f>SUM(H41:I41)</f>
         <v>0</v>
       </c>
-      <c r="K41" s="74"/>
+      <c r="K41" s="67"/>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B42" s="142"/>
-      <c r="C42" s="143"/>
-      <c r="D42" s="143"/>
+      <c r="B42" s="120"/>
+      <c r="C42" s="121"/>
+      <c r="D42" s="121"/>
       <c r="E42" s="8">
         <v>123456</v>
       </c>
@@ -3440,16 +3441,16 @@
       <c r="I42" s="8">
         <v>0</v>
       </c>
-      <c r="J42" s="73">
+      <c r="J42" s="66">
         <f>SUM(H42:I42)</f>
         <v>0</v>
       </c>
-      <c r="K42" s="74"/>
+      <c r="K42" s="67"/>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B43" s="142"/>
-      <c r="C43" s="143"/>
-      <c r="D43" s="143"/>
+      <c r="B43" s="120"/>
+      <c r="C43" s="121"/>
+      <c r="D43" s="121"/>
       <c r="E43" s="8">
         <v>123456</v>
       </c>
@@ -3465,52 +3466,52 @@
       <c r="I43" s="8">
         <v>0</v>
       </c>
-      <c r="J43" s="73">
+      <c r="J43" s="66">
         <f>SUM(H43:I43)</f>
         <v>0</v>
       </c>
-      <c r="K43" s="74"/>
+      <c r="K43" s="67"/>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B44" s="142"/>
-      <c r="C44" s="143"/>
-      <c r="D44" s="143"/>
-      <c r="E44" s="148"/>
-      <c r="F44" s="152"/>
-      <c r="G44" s="153"/>
-      <c r="H44" s="148"/>
-      <c r="I44" s="148"/>
-      <c r="K44" s="74"/>
+      <c r="B44" s="120"/>
+      <c r="C44" s="121"/>
+      <c r="D44" s="121"/>
+      <c r="E44" s="126"/>
+      <c r="F44" s="130"/>
+      <c r="G44" s="131"/>
+      <c r="H44" s="126"/>
+      <c r="I44" s="126"/>
+      <c r="K44" s="67"/>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B45" s="142">
+      <c r="B45" s="120">
         <v>7</v>
       </c>
-      <c r="C45" s="143">
+      <c r="C45" s="121">
         <v>100</v>
       </c>
-      <c r="D45" s="144" t="s">
+      <c r="D45" s="122" t="s">
         <v>27</v>
       </c>
-      <c r="E45" s="143"/>
-      <c r="F45" s="144" t="s">
+      <c r="E45" s="121"/>
+      <c r="F45" s="122" t="s">
         <v>28</v>
       </c>
-      <c r="G45" s="145">
+      <c r="G45" s="123">
         <v>888.8</v>
       </c>
-      <c r="H45" s="148"/>
-      <c r="I45" s="148"/>
-      <c r="J45" s="139"/>
-      <c r="K45" s="146">
+      <c r="H45" s="126"/>
+      <c r="I45" s="126"/>
+      <c r="J45" s="117"/>
+      <c r="K45" s="124">
         <f>IF(COUNTA(J46:J49)&lt;3,0,IF(COUNTA(J46:J49)=3,SUM(J46:J49),IF(SUM(J46:J49)&gt;0,SUM(J46:J49)-MINA(J46:J49),0)))</f>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B46" s="142"/>
-      <c r="C46" s="143"/>
-      <c r="D46" s="143"/>
+      <c r="B46" s="120"/>
+      <c r="C46" s="121"/>
+      <c r="D46" s="121"/>
       <c r="E46" s="8">
         <v>123456</v>
       </c>
@@ -3526,16 +3527,16 @@
       <c r="I46" s="8">
         <v>0</v>
       </c>
-      <c r="J46" s="73">
+      <c r="J46" s="66">
         <f>SUM(H46:I46)</f>
         <v>0</v>
       </c>
-      <c r="K46" s="74"/>
+      <c r="K46" s="67"/>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B47" s="142"/>
-      <c r="C47" s="143"/>
-      <c r="D47" s="143"/>
+      <c r="B47" s="120"/>
+      <c r="C47" s="121"/>
+      <c r="D47" s="121"/>
       <c r="E47" s="8">
         <v>123456</v>
       </c>
@@ -3551,16 +3552,16 @@
       <c r="I47" s="8">
         <v>0</v>
       </c>
-      <c r="J47" s="73">
+      <c r="J47" s="66">
         <f>SUM(H47:I47)</f>
         <v>0</v>
       </c>
-      <c r="K47" s="74"/>
+      <c r="K47" s="67"/>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B48" s="142"/>
-      <c r="C48" s="143"/>
-      <c r="D48" s="143"/>
+      <c r="B48" s="120"/>
+      <c r="C48" s="121"/>
+      <c r="D48" s="121"/>
       <c r="E48" s="8">
         <v>123456</v>
       </c>
@@ -3576,16 +3577,16 @@
       <c r="I48" s="8">
         <v>0</v>
       </c>
-      <c r="J48" s="73">
+      <c r="J48" s="66">
         <f>SUM(H48:I48)</f>
         <v>0</v>
       </c>
-      <c r="K48" s="74"/>
+      <c r="K48" s="67"/>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B49" s="142"/>
-      <c r="C49" s="143"/>
-      <c r="D49" s="143"/>
+      <c r="B49" s="120"/>
+      <c r="C49" s="121"/>
+      <c r="D49" s="121"/>
       <c r="E49" s="8">
         <v>123456</v>
       </c>
@@ -3601,52 +3602,52 @@
       <c r="I49" s="8">
         <v>0</v>
       </c>
-      <c r="J49" s="73">
+      <c r="J49" s="66">
         <f>SUM(H49:I49)</f>
         <v>0</v>
       </c>
-      <c r="K49" s="74"/>
+      <c r="K49" s="67"/>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B50" s="142"/>
-      <c r="C50" s="143"/>
-      <c r="D50" s="143"/>
-      <c r="E50" s="148"/>
-      <c r="F50" s="152"/>
-      <c r="G50" s="153"/>
-      <c r="H50" s="148"/>
-      <c r="I50" s="148"/>
-      <c r="K50" s="74"/>
+      <c r="B50" s="120"/>
+      <c r="C50" s="121"/>
+      <c r="D50" s="121"/>
+      <c r="E50" s="126"/>
+      <c r="F50" s="130"/>
+      <c r="G50" s="131"/>
+      <c r="H50" s="126"/>
+      <c r="I50" s="126"/>
+      <c r="K50" s="67"/>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B51" s="142">
+      <c r="B51" s="120">
         <v>8</v>
       </c>
-      <c r="C51" s="143">
+      <c r="C51" s="121">
         <v>100</v>
       </c>
-      <c r="D51" s="144" t="s">
+      <c r="D51" s="122" t="s">
         <v>25</v>
       </c>
-      <c r="E51" s="143"/>
-      <c r="F51" s="144" t="s">
+      <c r="E51" s="121"/>
+      <c r="F51" s="122" t="s">
         <v>26</v>
       </c>
-      <c r="G51" s="145">
+      <c r="G51" s="123">
         <v>888.8</v>
       </c>
-      <c r="H51" s="148"/>
-      <c r="I51" s="148"/>
-      <c r="J51" s="139"/>
-      <c r="K51" s="146">
+      <c r="H51" s="126"/>
+      <c r="I51" s="126"/>
+      <c r="J51" s="117"/>
+      <c r="K51" s="124">
         <f>IF(COUNTA(J52:J55)&lt;3,0,IF(COUNTA(J52:J55)=3,SUM(J52:J55),IF(SUM(J52:J55)&gt;0,SUM(J52:J55)-MINA(J52:J55),0)))</f>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B52" s="142"/>
-      <c r="C52" s="143"/>
-      <c r="D52" s="143"/>
+      <c r="B52" s="120"/>
+      <c r="C52" s="121"/>
+      <c r="D52" s="121"/>
       <c r="E52" s="8">
         <v>123456</v>
       </c>
@@ -3662,16 +3663,16 @@
       <c r="I52" s="8">
         <v>0</v>
       </c>
-      <c r="J52" s="73">
+      <c r="J52" s="66">
         <f>SUM(H52:I52)</f>
         <v>0</v>
       </c>
-      <c r="K52" s="74"/>
+      <c r="K52" s="67"/>
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B53" s="142"/>
-      <c r="C53" s="143"/>
-      <c r="D53" s="143"/>
+      <c r="B53" s="120"/>
+      <c r="C53" s="121"/>
+      <c r="D53" s="121"/>
       <c r="E53" s="8">
         <v>123456</v>
       </c>
@@ -3687,16 +3688,16 @@
       <c r="I53" s="8">
         <v>0</v>
       </c>
-      <c r="J53" s="73">
+      <c r="J53" s="66">
         <f>SUM(H53:I53)</f>
         <v>0</v>
       </c>
-      <c r="K53" s="74"/>
+      <c r="K53" s="67"/>
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B54" s="142"/>
-      <c r="C54" s="143"/>
-      <c r="D54" s="143"/>
+      <c r="B54" s="120"/>
+      <c r="C54" s="121"/>
+      <c r="D54" s="121"/>
       <c r="E54" s="8">
         <v>123456</v>
       </c>
@@ -3712,16 +3713,16 @@
       <c r="I54" s="8">
         <v>0</v>
       </c>
-      <c r="J54" s="73">
+      <c r="J54" s="66">
         <f>SUM(H54:I54)</f>
         <v>0</v>
       </c>
-      <c r="K54" s="74"/>
+      <c r="K54" s="67"/>
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B55" s="142"/>
-      <c r="C55" s="143"/>
-      <c r="D55" s="143"/>
+      <c r="B55" s="120"/>
+      <c r="C55" s="121"/>
+      <c r="D55" s="121"/>
       <c r="E55" s="8">
         <v>123456</v>
       </c>
@@ -3737,52 +3738,52 @@
       <c r="I55" s="8">
         <v>0</v>
       </c>
-      <c r="J55" s="73">
+      <c r="J55" s="66">
         <f>SUM(H55:I55)</f>
         <v>0</v>
       </c>
-      <c r="K55" s="74"/>
+      <c r="K55" s="67"/>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B56" s="142"/>
-      <c r="C56" s="143"/>
-      <c r="D56" s="143"/>
-      <c r="E56" s="148"/>
-      <c r="F56" s="152"/>
-      <c r="G56" s="153"/>
-      <c r="H56" s="148"/>
-      <c r="I56" s="148"/>
-      <c r="K56" s="74"/>
+      <c r="B56" s="120"/>
+      <c r="C56" s="121"/>
+      <c r="D56" s="121"/>
+      <c r="E56" s="126"/>
+      <c r="F56" s="130"/>
+      <c r="G56" s="131"/>
+      <c r="H56" s="126"/>
+      <c r="I56" s="126"/>
+      <c r="K56" s="67"/>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B57" s="142">
+      <c r="B57" s="120">
         <v>9</v>
       </c>
-      <c r="C57" s="143">
+      <c r="C57" s="121">
         <v>100</v>
       </c>
-      <c r="D57" s="144" t="s">
+      <c r="D57" s="122" t="s">
         <v>23</v>
       </c>
-      <c r="E57" s="143"/>
-      <c r="F57" s="144" t="s">
+      <c r="E57" s="121"/>
+      <c r="F57" s="122" t="s">
         <v>24</v>
       </c>
-      <c r="G57" s="145">
+      <c r="G57" s="123">
         <v>888.8</v>
       </c>
-      <c r="H57" s="148"/>
-      <c r="I57" s="148"/>
-      <c r="J57" s="139"/>
-      <c r="K57" s="146">
+      <c r="H57" s="126"/>
+      <c r="I57" s="126"/>
+      <c r="J57" s="117"/>
+      <c r="K57" s="124">
         <f>IF(COUNTA(J58:J61)&lt;3,0,IF(COUNTA(J58:J61)=3,SUM(J58:J61),IF(SUM(J58:J61)&gt;0,SUM(J58:J61)-MINA(J58:J61),0)))</f>
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B58" s="142"/>
-      <c r="C58" s="143"/>
-      <c r="D58" s="143"/>
+      <c r="B58" s="120"/>
+      <c r="C58" s="121"/>
+      <c r="D58" s="121"/>
       <c r="E58" s="8">
         <v>123456</v>
       </c>
@@ -3798,16 +3799,16 @@
       <c r="I58" s="8">
         <v>0</v>
       </c>
-      <c r="J58" s="73">
+      <c r="J58" s="66">
         <f>SUM(H58:I58)</f>
         <v>0</v>
       </c>
-      <c r="K58" s="74"/>
+      <c r="K58" s="67"/>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B59" s="142"/>
-      <c r="C59" s="143"/>
-      <c r="D59" s="143"/>
+      <c r="B59" s="120"/>
+      <c r="C59" s="121"/>
+      <c r="D59" s="121"/>
       <c r="E59" s="8">
         <v>123456</v>
       </c>
@@ -3823,16 +3824,16 @@
       <c r="I59" s="8">
         <v>0</v>
       </c>
-      <c r="J59" s="73">
+      <c r="J59" s="66">
         <f>SUM(H59:I59)</f>
         <v>0</v>
       </c>
-      <c r="K59" s="74"/>
+      <c r="K59" s="67"/>
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B60" s="142"/>
-      <c r="C60" s="143"/>
-      <c r="D60" s="143"/>
+      <c r="B60" s="120"/>
+      <c r="C60" s="121"/>
+      <c r="D60" s="121"/>
       <c r="E60" s="8">
         <v>123456</v>
       </c>
@@ -3848,16 +3849,16 @@
       <c r="I60" s="8">
         <v>0</v>
       </c>
-      <c r="J60" s="73">
+      <c r="J60" s="66">
         <f>SUM(H60:I60)</f>
         <v>0</v>
       </c>
-      <c r="K60" s="74"/>
+      <c r="K60" s="67"/>
     </row>
     <row r="61" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B61" s="142"/>
-      <c r="C61" s="143"/>
-      <c r="D61" s="143"/>
+      <c r="B61" s="120"/>
+      <c r="C61" s="121"/>
+      <c r="D61" s="121"/>
       <c r="E61" s="8">
         <v>123456</v>
       </c>
@@ -3873,53 +3874,53 @@
       <c r="I61" s="8">
         <v>0</v>
       </c>
-      <c r="J61" s="73">
+      <c r="J61" s="66">
         <f>SUM(H61:I61)</f>
         <v>0</v>
       </c>
-      <c r="K61" s="74"/>
+      <c r="K61" s="67"/>
     </row>
     <row r="62" spans="2:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="B62" s="149"/>
-      <c r="C62" s="95"/>
-      <c r="D62" s="95"/>
-      <c r="E62" s="95"/>
-      <c r="F62" s="95"/>
-      <c r="G62" s="150"/>
-      <c r="H62" s="148"/>
-      <c r="I62" s="148"/>
-      <c r="J62" s="95"/>
-      <c r="K62" s="151"/>
+      <c r="B62" s="127"/>
+      <c r="C62" s="82"/>
+      <c r="D62" s="82"/>
+      <c r="E62" s="82"/>
+      <c r="F62" s="82"/>
+      <c r="G62" s="128"/>
+      <c r="H62" s="126"/>
+      <c r="I62" s="126"/>
+      <c r="J62" s="82"/>
+      <c r="K62" s="129"/>
     </row>
     <row r="63" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B63" s="142">
+      <c r="B63" s="120">
         <v>10</v>
       </c>
-      <c r="C63" s="143">
+      <c r="C63" s="121">
         <v>100</v>
       </c>
-      <c r="D63" s="144" t="s">
+      <c r="D63" s="122" t="s">
         <v>21</v>
       </c>
-      <c r="E63" s="143"/>
-      <c r="F63" s="144" t="s">
+      <c r="E63" s="121"/>
+      <c r="F63" s="122" t="s">
         <v>22</v>
       </c>
-      <c r="G63" s="145">
+      <c r="G63" s="123">
         <v>888.8</v>
       </c>
-      <c r="H63" s="148"/>
-      <c r="I63" s="148"/>
-      <c r="J63" s="139"/>
-      <c r="K63" s="146">
+      <c r="H63" s="126"/>
+      <c r="I63" s="126"/>
+      <c r="J63" s="117"/>
+      <c r="K63" s="124">
         <f>IF(COUNTA(J64:J67)&lt;3,0,IF(COUNTA(J64:J67)=3,SUM(J64:J67),IF(SUM(J64:J67)&gt;0,SUM(J64:J67)-MINA(J64:J67),0)))</f>
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B64" s="142"/>
-      <c r="C64" s="143"/>
-      <c r="D64" s="143"/>
+      <c r="B64" s="120"/>
+      <c r="C64" s="121"/>
+      <c r="D64" s="121"/>
       <c r="E64" s="8">
         <v>123456</v>
       </c>
@@ -3935,16 +3936,16 @@
       <c r="I64" s="8">
         <v>0</v>
       </c>
-      <c r="J64" s="73">
+      <c r="J64" s="66">
         <f>SUM(H64:I64)</f>
         <v>0</v>
       </c>
-      <c r="K64" s="74"/>
+      <c r="K64" s="67"/>
     </row>
     <row r="65" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B65" s="142"/>
-      <c r="C65" s="143"/>
-      <c r="D65" s="143"/>
+      <c r="B65" s="120"/>
+      <c r="C65" s="121"/>
+      <c r="D65" s="121"/>
       <c r="E65" s="8">
         <v>123456</v>
       </c>
@@ -3960,16 +3961,16 @@
       <c r="I65" s="8">
         <v>0</v>
       </c>
-      <c r="J65" s="73">
+      <c r="J65" s="66">
         <f>SUM(H65:I65)</f>
         <v>0</v>
       </c>
-      <c r="K65" s="74"/>
+      <c r="K65" s="67"/>
     </row>
     <row r="66" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B66" s="142"/>
-      <c r="C66" s="143"/>
-      <c r="D66" s="143"/>
+      <c r="B66" s="120"/>
+      <c r="C66" s="121"/>
+      <c r="D66" s="121"/>
       <c r="E66" s="8">
         <v>123456</v>
       </c>
@@ -3985,16 +3986,16 @@
       <c r="I66" s="8">
         <v>0</v>
       </c>
-      <c r="J66" s="73">
+      <c r="J66" s="66">
         <f>SUM(H66:I66)</f>
         <v>0</v>
       </c>
-      <c r="K66" s="74"/>
+      <c r="K66" s="67"/>
     </row>
     <row r="67" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B67" s="142"/>
-      <c r="C67" s="143"/>
-      <c r="D67" s="143"/>
+      <c r="B67" s="120"/>
+      <c r="C67" s="121"/>
+      <c r="D67" s="121"/>
       <c r="E67" s="8">
         <v>123456</v>
       </c>
@@ -4010,47 +4011,47 @@
       <c r="I67" s="8">
         <v>0</v>
       </c>
-      <c r="J67" s="73">
+      <c r="J67" s="66">
         <f>SUM(H67:I67)</f>
         <v>0</v>
       </c>
-      <c r="K67" s="74"/>
+      <c r="K67" s="67"/>
     </row>
     <row r="68" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B68" s="138"/>
-      <c r="H68" s="148"/>
-      <c r="I68" s="148"/>
-      <c r="K68" s="74"/>
+      <c r="B68" s="116"/>
+      <c r="H68" s="126"/>
+      <c r="I68" s="126"/>
+      <c r="K68" s="67"/>
     </row>
     <row r="69" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B69" s="142">
+      <c r="B69" s="120">
         <v>11</v>
       </c>
-      <c r="C69" s="143">
+      <c r="C69" s="121">
         <v>100</v>
       </c>
-      <c r="D69" s="144" t="s">
+      <c r="D69" s="122" t="s">
         <v>20</v>
       </c>
-      <c r="E69" s="143"/>
-      <c r="F69" s="144" t="s">
+      <c r="E69" s="121"/>
+      <c r="F69" s="122" t="s">
         <v>19</v>
       </c>
-      <c r="G69" s="145">
+      <c r="G69" s="123">
         <v>888.8</v>
       </c>
-      <c r="H69" s="148"/>
-      <c r="I69" s="148"/>
-      <c r="J69" s="139"/>
-      <c r="K69" s="146">
+      <c r="H69" s="126"/>
+      <c r="I69" s="126"/>
+      <c r="J69" s="117"/>
+      <c r="K69" s="124">
         <f>IF(COUNTA(J70:J73)&lt;3,0,IF(COUNTA(J70:J73)=3,SUM(J70:J73),IF(SUM(J70:J73)&gt;0,SUM(J70:J73)-MINA(J70:J73),0)))</f>
         <v>0</v>
       </c>
     </row>
     <row r="70" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B70" s="142"/>
-      <c r="C70" s="143"/>
-      <c r="D70" s="143"/>
+      <c r="B70" s="120"/>
+      <c r="C70" s="121"/>
+      <c r="D70" s="121"/>
       <c r="E70" s="8">
         <v>123456</v>
       </c>
@@ -4066,16 +4067,16 @@
       <c r="I70" s="8">
         <v>0</v>
       </c>
-      <c r="J70" s="73">
+      <c r="J70" s="66">
         <f>SUM(H70:I70)</f>
         <v>0</v>
       </c>
-      <c r="K70" s="74"/>
+      <c r="K70" s="67"/>
     </row>
     <row r="71" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B71" s="142"/>
-      <c r="C71" s="143"/>
-      <c r="D71" s="143"/>
+      <c r="B71" s="120"/>
+      <c r="C71" s="121"/>
+      <c r="D71" s="121"/>
       <c r="E71" s="8">
         <v>123456</v>
       </c>
@@ -4091,16 +4092,16 @@
       <c r="I71" s="8">
         <v>0</v>
       </c>
-      <c r="J71" s="73">
+      <c r="J71" s="66">
         <f>SUM(H71:I71)</f>
         <v>0</v>
       </c>
-      <c r="K71" s="74"/>
+      <c r="K71" s="67"/>
     </row>
     <row r="72" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B72" s="142"/>
-      <c r="C72" s="143"/>
-      <c r="D72" s="143"/>
+      <c r="B72" s="120"/>
+      <c r="C72" s="121"/>
+      <c r="D72" s="121"/>
       <c r="E72" s="8">
         <v>123456</v>
       </c>
@@ -4116,16 +4117,16 @@
       <c r="I72" s="8">
         <v>0</v>
       </c>
-      <c r="J72" s="73">
+      <c r="J72" s="66">
         <f>SUM(H72:I72)</f>
         <v>0</v>
       </c>
-      <c r="K72" s="74"/>
+      <c r="K72" s="67"/>
     </row>
     <row r="73" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B73" s="142"/>
-      <c r="C73" s="143"/>
-      <c r="D73" s="143"/>
+      <c r="B73" s="120"/>
+      <c r="C73" s="121"/>
+      <c r="D73" s="121"/>
       <c r="E73" s="8">
         <v>123456</v>
       </c>
@@ -4141,47 +4142,47 @@
       <c r="I73" s="8">
         <v>0</v>
       </c>
-      <c r="J73" s="73">
+      <c r="J73" s="66">
         <f>SUM(H73:I73)</f>
         <v>0</v>
       </c>
-      <c r="K73" s="74"/>
+      <c r="K73" s="67"/>
     </row>
     <row r="74" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B74" s="138"/>
-      <c r="H74" s="148"/>
-      <c r="I74" s="148"/>
-      <c r="K74" s="74"/>
+      <c r="B74" s="116"/>
+      <c r="H74" s="126"/>
+      <c r="I74" s="126"/>
+      <c r="K74" s="67"/>
     </row>
     <row r="75" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B75" s="142">
+      <c r="B75" s="120">
         <v>12</v>
       </c>
-      <c r="C75" s="143">
+      <c r="C75" s="121">
         <v>100</v>
       </c>
-      <c r="D75" s="144" t="s">
+      <c r="D75" s="122" t="s">
         <v>17</v>
       </c>
-      <c r="E75" s="143"/>
-      <c r="F75" s="144" t="s">
+      <c r="E75" s="121"/>
+      <c r="F75" s="122" t="s">
         <v>18</v>
       </c>
-      <c r="G75" s="145">
+      <c r="G75" s="123">
         <v>888.8</v>
       </c>
-      <c r="H75" s="148"/>
-      <c r="I75" s="148"/>
-      <c r="J75" s="139"/>
-      <c r="K75" s="146">
+      <c r="H75" s="126"/>
+      <c r="I75" s="126"/>
+      <c r="J75" s="117"/>
+      <c r="K75" s="124">
         <f>IF(COUNTA(J76:J79)&lt;3,0,IF(COUNTA(J76:J79)=3,SUM(J76:J79),IF(SUM(J76:J79)&gt;0,SUM(J76:J79)-MINA(J76:J79),0)))</f>
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B76" s="142"/>
-      <c r="C76" s="143"/>
-      <c r="D76" s="143"/>
+      <c r="B76" s="120"/>
+      <c r="C76" s="121"/>
+      <c r="D76" s="121"/>
       <c r="E76" s="8">
         <v>123456</v>
       </c>
@@ -4197,16 +4198,16 @@
       <c r="I76" s="8">
         <v>0</v>
       </c>
-      <c r="J76" s="73">
+      <c r="J76" s="66">
         <f>SUM(H76:I76)</f>
         <v>0</v>
       </c>
-      <c r="K76" s="74"/>
+      <c r="K76" s="67"/>
     </row>
     <row r="77" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B77" s="142"/>
-      <c r="C77" s="143"/>
-      <c r="D77" s="143"/>
+      <c r="B77" s="120"/>
+      <c r="C77" s="121"/>
+      <c r="D77" s="121"/>
       <c r="E77" s="8">
         <v>123456</v>
       </c>
@@ -4222,16 +4223,16 @@
       <c r="I77" s="8">
         <v>0</v>
       </c>
-      <c r="J77" s="73">
+      <c r="J77" s="66">
         <f>SUM(H77:I77)</f>
         <v>0</v>
       </c>
-      <c r="K77" s="74"/>
+      <c r="K77" s="67"/>
     </row>
     <row r="78" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B78" s="142"/>
-      <c r="C78" s="143"/>
-      <c r="D78" s="143"/>
+      <c r="B78" s="120"/>
+      <c r="C78" s="121"/>
+      <c r="D78" s="121"/>
       <c r="E78" s="8">
         <v>123456</v>
       </c>
@@ -4247,16 +4248,16 @@
       <c r="I78" s="8">
         <v>0</v>
       </c>
-      <c r="J78" s="73">
+      <c r="J78" s="66">
         <f>SUM(H78:I78)</f>
         <v>0</v>
       </c>
-      <c r="K78" s="74"/>
+      <c r="K78" s="67"/>
     </row>
     <row r="79" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B79" s="142"/>
-      <c r="C79" s="143"/>
-      <c r="D79" s="143"/>
+      <c r="B79" s="120"/>
+      <c r="C79" s="121"/>
+      <c r="D79" s="121"/>
       <c r="E79" s="8">
         <v>123456</v>
       </c>
@@ -4272,27 +4273,27 @@
       <c r="I79" s="8">
         <v>0</v>
       </c>
-      <c r="J79" s="73">
+      <c r="J79" s="66">
         <f>SUM(H79:I79)</f>
         <v>0</v>
       </c>
-      <c r="K79" s="74"/>
+      <c r="K79" s="67"/>
     </row>
     <row r="80" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="156"/>
-      <c r="C80" s="157"/>
-      <c r="D80" s="157"/>
-      <c r="E80" s="158"/>
-      <c r="F80" s="158"/>
-      <c r="G80" s="159"/>
-      <c r="H80" s="154"/>
-      <c r="I80" s="154"/>
-      <c r="J80" s="154"/>
-      <c r="K80" s="155"/>
+      <c r="B80" s="134"/>
+      <c r="C80" s="135"/>
+      <c r="D80" s="135"/>
+      <c r="E80" s="136"/>
+      <c r="F80" s="136"/>
+      <c r="G80" s="137"/>
+      <c r="H80" s="132"/>
+      <c r="I80" s="132"/>
+      <c r="J80" s="132"/>
+      <c r="K80" s="133"/>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.2"/>
     <row r="82" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B82" s="147" t="s">
+      <c r="B82" s="125" t="s">
         <v>47</v>
       </c>
     </row>
@@ -4333,304 +4334,304 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.44140625" style="95" customWidth="1"/>
-    <col min="2" max="2" width="5.77734375" style="96" customWidth="1"/>
-    <col min="3" max="4" width="29.5546875" style="95" customWidth="1"/>
-    <col min="5" max="8" width="5.77734375" style="95" customWidth="1"/>
-    <col min="9" max="9" width="1.88671875" style="95" customWidth="1"/>
-    <col min="10" max="13" width="5.77734375" style="95" customWidth="1"/>
-    <col min="14" max="14" width="1.88671875" style="95" customWidth="1"/>
-    <col min="15" max="21" width="5.77734375" style="95" customWidth="1"/>
-    <col min="22" max="22" width="2.109375" style="95" customWidth="1"/>
-    <col min="23" max="23" width="10.33203125" style="95" customWidth="1"/>
-    <col min="24" max="24" width="0.88671875" style="95" customWidth="1"/>
-    <col min="25" max="25" width="3.44140625" style="95" customWidth="1"/>
-    <col min="26" max="26" width="3" style="95" customWidth="1"/>
-    <col min="27" max="16384" width="9.77734375" style="95" hidden="1"/>
+    <col min="1" max="1" width="4.44140625" style="82" customWidth="1"/>
+    <col min="2" max="2" width="5.77734375" style="83" customWidth="1"/>
+    <col min="3" max="4" width="29.5546875" style="82" customWidth="1"/>
+    <col min="5" max="8" width="5.77734375" style="82" customWidth="1"/>
+    <col min="9" max="9" width="1.88671875" style="82" customWidth="1"/>
+    <col min="10" max="13" width="5.77734375" style="82" customWidth="1"/>
+    <col min="14" max="14" width="1.88671875" style="82" customWidth="1"/>
+    <col min="15" max="21" width="5.77734375" style="82" customWidth="1"/>
+    <col min="22" max="22" width="2.109375" style="82" customWidth="1"/>
+    <col min="23" max="23" width="10.33203125" style="82" customWidth="1"/>
+    <col min="24" max="24" width="0.88671875" style="82" customWidth="1"/>
+    <col min="25" max="25" width="3.44140625" style="82" customWidth="1"/>
+    <col min="26" max="26" width="3" style="82" customWidth="1"/>
+    <col min="27" max="16384" width="9.77734375" style="82" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="95"/>
-      <c r="B1" s="96"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="95"/>
-      <c r="J1" s="95"/>
-      <c r="K1" s="95"/>
-      <c r="L1" s="95"/>
-      <c r="M1" s="95"/>
-      <c r="N1" s="95"/>
-      <c r="O1" s="95"/>
-      <c r="P1" s="95"/>
-      <c r="Q1" s="95"/>
-      <c r="R1" s="95"/>
-      <c r="S1" s="95"/>
-      <c r="T1" s="95"/>
-      <c r="U1" s="95"/>
-      <c r="V1" s="95"/>
-      <c r="W1" s="95"/>
-      <c r="X1" s="95"/>
-      <c r="Y1" s="95"/>
-      <c r="Z1" s="95"/>
+      <c r="A1" s="82"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+      <c r="L1" s="82"/>
+      <c r="M1" s="82"/>
+      <c r="N1" s="82"/>
+      <c r="O1" s="82"/>
+      <c r="P1" s="82"/>
+      <c r="Q1" s="82"/>
+      <c r="R1" s="82"/>
+      <c r="S1" s="82"/>
+      <c r="T1" s="82"/>
+      <c r="U1" s="82"/>
+      <c r="V1" s="82"/>
+      <c r="W1" s="82"/>
+      <c r="X1" s="82"/>
+      <c r="Y1" s="82"/>
+      <c r="Z1" s="82"/>
     </row>
     <row r="2" spans="1:28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="95"/>
-      <c r="B2" s="102" t="str">
+      <c r="A2" s="82"/>
+      <c r="B2" s="154" t="str">
         <f>'Deelnemers en Scores'!B2</f>
         <v>BK 25m1pijl Teams, Klasse: komt hier</v>
       </c>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
-      <c r="O2" s="103"/>
-      <c r="P2" s="103"/>
-      <c r="Q2" s="103"/>
-      <c r="R2" s="103"/>
-      <c r="S2" s="103"/>
-      <c r="T2" s="103"/>
-      <c r="U2" s="103"/>
-      <c r="V2" s="103"/>
-      <c r="W2" s="104"/>
-      <c r="X2" s="95"/>
-      <c r="Y2" s="95"/>
-      <c r="Z2" s="95"/>
+      <c r="C2" s="155"/>
+      <c r="D2" s="155"/>
+      <c r="E2" s="155"/>
+      <c r="F2" s="155"/>
+      <c r="G2" s="155"/>
+      <c r="H2" s="155"/>
+      <c r="I2" s="155"/>
+      <c r="J2" s="155"/>
+      <c r="K2" s="155"/>
+      <c r="L2" s="155"/>
+      <c r="M2" s="155"/>
+      <c r="N2" s="155"/>
+      <c r="O2" s="155"/>
+      <c r="P2" s="155"/>
+      <c r="Q2" s="155"/>
+      <c r="R2" s="155"/>
+      <c r="S2" s="155"/>
+      <c r="T2" s="155"/>
+      <c r="U2" s="155"/>
+      <c r="V2" s="155"/>
+      <c r="W2" s="156"/>
+      <c r="X2" s="82"/>
+      <c r="Y2" s="82"/>
+      <c r="Z2" s="82"/>
     </row>
     <row r="3" spans="1:28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="95"/>
-      <c r="B3" s="96"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="95"/>
-      <c r="H3" s="95"/>
-      <c r="I3" s="95"/>
-      <c r="J3" s="95"/>
-      <c r="K3" s="95"/>
-      <c r="L3" s="95"/>
-      <c r="M3" s="95"/>
-      <c r="N3" s="95"/>
-      <c r="O3" s="95"/>
-      <c r="P3" s="95"/>
-      <c r="Q3" s="95"/>
-      <c r="R3" s="95"/>
-      <c r="S3" s="95"/>
-      <c r="T3" s="95"/>
-      <c r="U3" s="95"/>
-      <c r="V3" s="95"/>
-      <c r="W3" s="95"/>
-      <c r="X3" s="95"/>
-      <c r="Y3" s="95"/>
-      <c r="Z3" s="95"/>
+      <c r="A3" s="82"/>
+      <c r="B3" s="83"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
+      <c r="L3" s="82"/>
+      <c r="M3" s="82"/>
+      <c r="N3" s="82"/>
+      <c r="O3" s="82"/>
+      <c r="P3" s="82"/>
+      <c r="Q3" s="82"/>
+      <c r="R3" s="82"/>
+      <c r="S3" s="82"/>
+      <c r="T3" s="82"/>
+      <c r="U3" s="82"/>
+      <c r="V3" s="82"/>
+      <c r="W3" s="82"/>
+      <c r="X3" s="82"/>
+      <c r="Y3" s="82"/>
+      <c r="Z3" s="82"/>
     </row>
     <row r="4" spans="1:28" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="95"/>
-      <c r="B4" s="95"/>
-      <c r="C4" s="95"/>
-      <c r="D4" s="95"/>
-      <c r="E4" s="110"/>
-      <c r="F4" s="95"/>
-      <c r="G4" s="95"/>
-      <c r="H4" s="95"/>
-      <c r="I4" s="95"/>
-      <c r="J4" s="95"/>
-      <c r="K4" s="95"/>
-      <c r="L4" s="95"/>
-      <c r="M4" s="95"/>
-      <c r="N4" s="95"/>
-      <c r="O4" s="111" t="s">
+      <c r="A4" s="82"/>
+      <c r="B4" s="82"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="93"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82"/>
+      <c r="I4" s="82"/>
+      <c r="J4" s="82"/>
+      <c r="K4" s="82"/>
+      <c r="L4" s="82"/>
+      <c r="M4" s="82"/>
+      <c r="N4" s="82"/>
+      <c r="O4" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="P4" s="112" t="str">
+      <c r="P4" s="157" t="str">
         <f>'Deelnemers en Scores'!H4</f>
         <v>yyyy-mm-dd</v>
       </c>
-      <c r="Q4" s="113"/>
-      <c r="R4" s="113"/>
-      <c r="S4" s="113"/>
-      <c r="T4" s="113"/>
-      <c r="U4" s="113"/>
-      <c r="V4" s="114"/>
-      <c r="W4" s="115"/>
-      <c r="X4" s="95"/>
-      <c r="Y4" s="95"/>
-      <c r="Z4" s="95"/>
+      <c r="Q4" s="158"/>
+      <c r="R4" s="158"/>
+      <c r="S4" s="158"/>
+      <c r="T4" s="158"/>
+      <c r="U4" s="158"/>
+      <c r="V4" s="95"/>
+      <c r="W4" s="96"/>
+      <c r="X4" s="82"/>
+      <c r="Y4" s="82"/>
+      <c r="Z4" s="82"/>
     </row>
     <row r="5" spans="1:28" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="95"/>
-      <c r="B5" s="96"/>
-      <c r="C5" s="95"/>
-      <c r="D5" s="95"/>
-      <c r="E5" s="95"/>
-      <c r="F5" s="95"/>
-      <c r="G5" s="95"/>
-      <c r="H5" s="95"/>
-      <c r="I5" s="95"/>
-      <c r="J5" s="95"/>
-      <c r="K5" s="95"/>
-      <c r="L5" s="95"/>
-      <c r="M5" s="95"/>
-      <c r="N5" s="95"/>
-      <c r="O5" s="95"/>
-      <c r="P5" s="95"/>
-      <c r="Q5" s="95"/>
-      <c r="R5" s="95"/>
-      <c r="S5" s="95"/>
-      <c r="T5" s="95"/>
-      <c r="U5" s="95"/>
-      <c r="V5" s="95"/>
-      <c r="W5" s="95"/>
-      <c r="X5" s="95"/>
-      <c r="Y5" s="95"/>
-      <c r="Z5" s="95"/>
+      <c r="A5" s="82"/>
+      <c r="B5" s="83"/>
+      <c r="C5" s="82"/>
+      <c r="D5" s="82"/>
+      <c r="E5" s="82"/>
+      <c r="F5" s="82"/>
+      <c r="G5" s="82"/>
+      <c r="H5" s="82"/>
+      <c r="I5" s="82"/>
+      <c r="J5" s="82"/>
+      <c r="K5" s="82"/>
+      <c r="L5" s="82"/>
+      <c r="M5" s="82"/>
+      <c r="N5" s="82"/>
+      <c r="O5" s="82"/>
+      <c r="P5" s="82"/>
+      <c r="Q5" s="82"/>
+      <c r="R5" s="82"/>
+      <c r="S5" s="82"/>
+      <c r="T5" s="82"/>
+      <c r="U5" s="82"/>
+      <c r="V5" s="82"/>
+      <c r="W5" s="82"/>
+      <c r="X5" s="82"/>
+      <c r="Y5" s="82"/>
+      <c r="Z5" s="82"/>
     </row>
     <row r="6" spans="1:28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="95"/>
-      <c r="B6" s="96"/>
-      <c r="C6" s="95"/>
-      <c r="D6" s="95"/>
-      <c r="E6" s="95"/>
-      <c r="F6" s="95"/>
-      <c r="G6" s="95"/>
-      <c r="H6" s="95"/>
-      <c r="I6" s="95"/>
-      <c r="J6" s="95"/>
-      <c r="K6" s="95"/>
-      <c r="L6" s="95"/>
-      <c r="M6" s="95"/>
-      <c r="N6" s="95"/>
-      <c r="O6" s="95"/>
-      <c r="P6" s="95"/>
-      <c r="Q6" s="95"/>
-      <c r="R6" s="95"/>
-      <c r="S6" s="95"/>
-      <c r="T6" s="95"/>
-      <c r="U6" s="95"/>
-      <c r="V6" s="95"/>
-      <c r="W6" s="95"/>
-      <c r="X6" s="95"/>
-      <c r="Y6" s="95"/>
-      <c r="Z6" s="95"/>
+      <c r="A6" s="82"/>
+      <c r="B6" s="83"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="82"/>
+      <c r="G6" s="82"/>
+      <c r="H6" s="82"/>
+      <c r="I6" s="82"/>
+      <c r="J6" s="82"/>
+      <c r="K6" s="82"/>
+      <c r="L6" s="82"/>
+      <c r="M6" s="82"/>
+      <c r="N6" s="82"/>
+      <c r="O6" s="82"/>
+      <c r="P6" s="82"/>
+      <c r="Q6" s="82"/>
+      <c r="R6" s="82"/>
+      <c r="S6" s="82"/>
+      <c r="T6" s="82"/>
+      <c r="U6" s="82"/>
+      <c r="V6" s="82"/>
+      <c r="W6" s="82"/>
+      <c r="X6" s="82"/>
+      <c r="Y6" s="82"/>
+      <c r="Z6" s="82"/>
     </row>
     <row r="7" spans="1:28" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="95"/>
-      <c r="B7" s="116"/>
-      <c r="C7" s="117"/>
-      <c r="D7" s="118"/>
-      <c r="E7" s="119" t="s">
+      <c r="A7" s="82"/>
+      <c r="B7" s="97"/>
+      <c r="C7" s="98"/>
+      <c r="D7" s="99"/>
+      <c r="E7" s="152" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="120"/>
-      <c r="G7" s="120"/>
-      <c r="H7" s="120"/>
-      <c r="I7" s="121"/>
-      <c r="J7" s="120" t="s">
+      <c r="F7" s="159"/>
+      <c r="G7" s="159"/>
+      <c r="H7" s="159"/>
+      <c r="I7" s="101"/>
+      <c r="J7" s="159" t="s">
         <v>36</v>
       </c>
-      <c r="K7" s="120"/>
-      <c r="L7" s="120"/>
-      <c r="M7" s="122"/>
-      <c r="N7" s="123"/>
-      <c r="O7" s="119" t="s">
+      <c r="K7" s="159"/>
+      <c r="L7" s="159"/>
+      <c r="M7" s="153"/>
+      <c r="N7" s="100"/>
+      <c r="O7" s="152" t="s">
         <v>37</v>
       </c>
-      <c r="P7" s="120"/>
-      <c r="Q7" s="120"/>
-      <c r="R7" s="122"/>
-      <c r="S7" s="123" t="s">
+      <c r="P7" s="159"/>
+      <c r="Q7" s="159"/>
+      <c r="R7" s="153"/>
+      <c r="S7" s="100" t="s">
         <v>91</v>
       </c>
-      <c r="T7" s="119" t="s">
+      <c r="T7" s="152" t="s">
         <v>90</v>
       </c>
-      <c r="U7" s="122"/>
-      <c r="V7" s="121"/>
-      <c r="W7" s="124" t="s">
+      <c r="U7" s="153"/>
+      <c r="V7" s="101"/>
+      <c r="W7" s="102" t="s">
         <v>89</v>
       </c>
-      <c r="X7" s="95"/>
-      <c r="Y7" s="95"/>
-      <c r="Z7" s="95"/>
+      <c r="X7" s="82"/>
+      <c r="Y7" s="82"/>
+      <c r="Z7" s="82"/>
     </row>
     <row r="8" spans="1:28" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="96"/>
-      <c r="B8" s="125" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="126" t="s">
+      <c r="A8" s="83"/>
+      <c r="B8" s="103" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="104" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="127" t="s">
+      <c r="D8" s="105" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="128">
+      <c r="E8" s="106">
         <v>1</v>
       </c>
-      <c r="F8" s="129">
+      <c r="F8" s="107">
         <v>2</v>
       </c>
-      <c r="G8" s="129">
+      <c r="G8" s="107">
         <v>3</v>
       </c>
-      <c r="H8" s="130">
+      <c r="H8" s="108">
         <v>4</v>
       </c>
-      <c r="I8" s="131"/>
-      <c r="J8" s="128">
+      <c r="I8" s="109"/>
+      <c r="J8" s="106">
         <v>1</v>
       </c>
-      <c r="K8" s="129">
+      <c r="K8" s="107">
         <v>2</v>
       </c>
-      <c r="L8" s="129">
+      <c r="L8" s="107">
         <v>3</v>
       </c>
-      <c r="M8" s="132">
+      <c r="M8" s="110">
         <v>4</v>
       </c>
-      <c r="N8" s="131"/>
-      <c r="O8" s="128">
+      <c r="N8" s="109"/>
+      <c r="O8" s="106">
         <v>1</v>
       </c>
-      <c r="P8" s="129">
+      <c r="P8" s="107">
         <v>2</v>
       </c>
-      <c r="Q8" s="129">
+      <c r="Q8" s="107">
         <v>3</v>
       </c>
-      <c r="R8" s="132">
+      <c r="R8" s="110">
         <v>4</v>
       </c>
-      <c r="S8" s="133" t="s">
+      <c r="S8" s="111" t="s">
         <v>92</v>
       </c>
-      <c r="T8" s="134" t="s">
+      <c r="T8" s="112" t="s">
         <v>49</v>
       </c>
-      <c r="U8" s="135" t="s">
+      <c r="U8" s="113" t="s">
         <v>50</v>
       </c>
-      <c r="V8" s="131"/>
-      <c r="W8" s="133"/>
-      <c r="X8" s="95"/>
-      <c r="Y8" s="95"/>
-      <c r="Z8" s="95"/>
+      <c r="V8" s="109"/>
+      <c r="W8" s="111"/>
+      <c r="X8" s="82"/>
+      <c r="Y8" s="82"/>
+      <c r="Z8" s="82"/>
     </row>
     <row r="9" spans="1:28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="96"/>
+      <c r="A9" s="83"/>
       <c r="B9" s="51">
         <f>IF('Deelnemers en Scores'!B9&gt;0,'Deelnemers en Scores'!B9,"")</f>
         <v>1</v>
@@ -4659,7 +4660,7 @@
         <f>IF('Deelnemers en Scores'!H13=0,"",'Deelnemers en Scores'!H13)</f>
         <v/>
       </c>
-      <c r="I9" s="105"/>
+      <c r="I9" s="88"/>
       <c r="J9" s="54" t="str">
         <f>IF('Deelnemers en Scores'!I10=0,"",'Deelnemers en Scores'!I10)</f>
         <v/>
@@ -4676,46 +4677,46 @@
         <f>IF('Deelnemers en Scores'!I13=0,"",'Deelnemers en Scores'!I13)</f>
         <v/>
       </c>
-      <c r="N9" s="105"/>
+      <c r="N9" s="88"/>
       <c r="O9" s="56" t="str">
-        <f>IF(ISNUMBER(J9),E9+J9,"")</f>
+        <f t="shared" ref="O9:O20" si="0">IF(ISNUMBER(J9),E9+J9,"")</f>
         <v/>
       </c>
       <c r="P9" s="57" t="str">
-        <f>IF(ISNUMBER(K9),F9+K9,"")</f>
+        <f t="shared" ref="P9:P20" si="1">IF(ISNUMBER(K9),F9+K9,"")</f>
         <v/>
       </c>
       <c r="Q9" s="57" t="str">
-        <f>IF(ISNUMBER(L9),G9+L9,"")</f>
+        <f t="shared" ref="Q9:Q20" si="2">IF(ISNUMBER(L9),G9+L9,"")</f>
         <v/>
       </c>
       <c r="R9" s="58" t="str">
-        <f>IF(ISNUMBER(M9),H9+M9,"")</f>
+        <f t="shared" ref="R9:R20" si="3">IF(ISNUMBER(M9),H9+M9,"")</f>
         <v/>
       </c>
       <c r="S9" s="60">
-        <f>IF(COUNT(O9:R9)&lt;4,SUM(O9:R9),SUM(O9:R9)-MIN(O9:R9))</f>
+        <f t="shared" ref="S9:S20" si="4">IF(COUNT(O9:R9)&lt;4,SUM(O9:R9),SUM(O9:R9)-MIN(O9:R9))</f>
         <v>0</v>
       </c>
       <c r="T9" s="56">
-        <f>LARGE(O9:R9,1)</f>
+        <f t="shared" ref="T9:T20" si="5">LARGE(O9:R9,1)</f>
         <v>0</v>
       </c>
       <c r="U9" s="58">
-        <f>LARGE(O9:R9,2)</f>
-        <v>0</v>
-      </c>
-      <c r="V9" s="105"/>
+        <f t="shared" ref="U9:U20" si="6">LARGE(O9:R9,2)</f>
+        <v>0</v>
+      </c>
+      <c r="V9" s="88"/>
       <c r="W9" s="59">
-        <f>S9+T9/10000+U9/10000000</f>
-        <v>0</v>
-      </c>
-      <c r="X9" s="99"/>
-      <c r="Y9" s="136" t="str">
+        <f>S9+D23</f>
+        <v>0</v>
+      </c>
+      <c r="X9" s="86"/>
+      <c r="Y9" s="114" t="str">
         <f>IF(W9&gt;0,IF(W9=W8,Y8,ROW()-ROW($Y$8)),"")</f>
         <v/>
       </c>
-      <c r="Z9" s="137" t="str">
+      <c r="Z9" s="115" t="str">
         <f>IF(Y9&lt;&gt;"","e","")</f>
         <v/>
       </c>
@@ -4723,7 +4724,7 @@
       <c r="AB9" s="40"/>
     </row>
     <row r="10" spans="1:28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="96"/>
+      <c r="A10" s="83"/>
       <c r="B10" s="49">
         <f>IF('Deelnemers en Scores'!B27&gt;0,'Deelnemers en Scores'!B27,"")</f>
         <v>4</v>
@@ -4752,7 +4753,7 @@
         <f>IF('Deelnemers en Scores'!H31=0,"",'Deelnemers en Scores'!H31)</f>
         <v/>
       </c>
-      <c r="I10" s="106"/>
+      <c r="I10" s="89"/>
       <c r="J10" s="18" t="str">
         <f>IF('Deelnemers en Scores'!I28=0,"",'Deelnemers en Scores'!I28)</f>
         <v/>
@@ -4769,52 +4770,52 @@
         <f>IF('Deelnemers en Scores'!I31=0,"",'Deelnemers en Scores'!I31)</f>
         <v/>
       </c>
-      <c r="N10" s="106"/>
+      <c r="N10" s="89"/>
       <c r="O10" s="19" t="str">
-        <f>IF(ISNUMBER(J10),E10+J10,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="P10" s="20" t="str">
-        <f>IF(ISNUMBER(K10),F10+K10,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q10" s="20" t="str">
-        <f>IF(ISNUMBER(L10),G10+L10,"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="R10" s="21" t="str">
-        <f>IF(ISNUMBER(M10),H10+M10,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S10" s="60">
-        <f>IF(COUNT(O10:R10)&lt;4,SUM(O10:R10),SUM(O10:R10)-MIN(O10:R10))</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T10" s="56">
-        <f>LARGE(O10:R10,1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U10" s="58">
-        <f>LARGE(O10:R10,2)</f>
-        <v>0</v>
-      </c>
-      <c r="V10" s="106"/>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V10" s="89"/>
       <c r="W10" s="59">
-        <f>S10+T10/10000+U10/10000000</f>
-        <v>0</v>
-      </c>
-      <c r="X10" s="99"/>
-      <c r="Y10" s="136" t="str">
-        <f t="shared" ref="Y10:Y20" si="0">IF(W10&gt;0,IF(W10=W9,Y9,ROW()-ROW($Y$8)),"")</f>
-        <v/>
-      </c>
-      <c r="Z10" s="137" t="str">
-        <f t="shared" ref="Z10:Z20" si="1">IF(Y10&lt;&gt;"","e","")</f>
+        <f t="shared" ref="W10:W20" si="7">S10+T10/10000+U10/10000000</f>
+        <v>0</v>
+      </c>
+      <c r="X10" s="86"/>
+      <c r="Y10" s="114" t="str">
+        <f t="shared" ref="Y10:Y20" si="8">IF(W10&gt;0,IF(W10=W9,Y9,ROW()-ROW($Y$8)),"")</f>
+        <v/>
+      </c>
+      <c r="Z10" s="115" t="str">
+        <f t="shared" ref="Z10:Z20" si="9">IF(Y10&lt;&gt;"","e","")</f>
         <v/>
       </c>
     </row>
     <row r="11" spans="1:28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="96"/>
+      <c r="A11" s="83"/>
       <c r="B11" s="49">
         <f>IF('Deelnemers en Scores'!B15&gt;0,'Deelnemers en Scores'!B15,"")</f>
         <v>2</v>
@@ -4843,7 +4844,7 @@
         <f>IF('Deelnemers en Scores'!H19=0,"",'Deelnemers en Scores'!H19)</f>
         <v/>
       </c>
-      <c r="I11" s="106"/>
+      <c r="I11" s="89"/>
       <c r="J11" s="18" t="str">
         <f>IF('Deelnemers en Scores'!I16=0,"",'Deelnemers en Scores'!I16)</f>
         <v/>
@@ -4860,52 +4861,52 @@
         <f>IF('Deelnemers en Scores'!I19=0,"",'Deelnemers en Scores'!I19)</f>
         <v/>
       </c>
-      <c r="N11" s="106"/>
+      <c r="N11" s="89"/>
       <c r="O11" s="19" t="str">
-        <f>IF(ISNUMBER(J11),E11+J11,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="P11" s="20" t="str">
-        <f>IF(ISNUMBER(K11),F11+K11,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q11" s="20" t="str">
-        <f>IF(ISNUMBER(L11),G11+L11,"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="R11" s="21" t="str">
-        <f>IF(ISNUMBER(M11),H11+M11,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S11" s="60">
-        <f>IF(COUNT(O11:R11)&lt;4,SUM(O11:R11),SUM(O11:R11)-MIN(O11:R11))</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T11" s="56">
-        <f>LARGE(O11:R11,1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U11" s="58">
-        <f>LARGE(O11:R11,2)</f>
-        <v>0</v>
-      </c>
-      <c r="V11" s="106"/>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V11" s="89"/>
       <c r="W11" s="59">
-        <f>S11+T11/10000+U11/10000000</f>
-        <v>0</v>
-      </c>
-      <c r="X11" s="99"/>
-      <c r="Y11" s="136" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="Z11" s="137" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X11" s="86"/>
+      <c r="Y11" s="114" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="Z11" s="115" t="str">
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
     <row r="12" spans="1:28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="96"/>
+      <c r="A12" s="83"/>
       <c r="B12" s="49">
         <f>IF('Deelnemers en Scores'!B21&gt;0,'Deelnemers en Scores'!B21,"")</f>
         <v>3</v>
@@ -4934,7 +4935,7 @@
         <f>IF('Deelnemers en Scores'!H25=0,"",'Deelnemers en Scores'!H25)</f>
         <v/>
       </c>
-      <c r="I12" s="106"/>
+      <c r="I12" s="89"/>
       <c r="J12" s="18" t="str">
         <f>IF('Deelnemers en Scores'!I22=0,"",'Deelnemers en Scores'!I22)</f>
         <v/>
@@ -4951,52 +4952,52 @@
         <f>IF('Deelnemers en Scores'!I25=0,"",'Deelnemers en Scores'!I25)</f>
         <v/>
       </c>
-      <c r="N12" s="106"/>
+      <c r="N12" s="89"/>
       <c r="O12" s="19" t="str">
-        <f>IF(ISNUMBER(J12),E12+J12,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="P12" s="20" t="str">
-        <f>IF(ISNUMBER(K12),F12+K12,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q12" s="20" t="str">
-        <f>IF(ISNUMBER(L12),G12+L12,"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="R12" s="21" t="str">
-        <f>IF(ISNUMBER(M12),H12+M12,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S12" s="60">
-        <f>IF(COUNT(O12:R12)&lt;4,SUM(O12:R12),SUM(O12:R12)-MIN(O12:R12))</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T12" s="56">
-        <f>LARGE(O12:R12,1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U12" s="58">
-        <f>LARGE(O12:R12,2)</f>
-        <v>0</v>
-      </c>
-      <c r="V12" s="106"/>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V12" s="89"/>
       <c r="W12" s="59">
-        <f>S12+T12/10000+U12/10000000</f>
-        <v>0</v>
-      </c>
-      <c r="X12" s="99"/>
-      <c r="Y12" s="136" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="Z12" s="137" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X12" s="86"/>
+      <c r="Y12" s="114" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="Z12" s="115" t="str">
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
     <row r="13" spans="1:28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="96"/>
+      <c r="A13" s="83"/>
       <c r="B13" s="49">
         <f>IF('Deelnemers en Scores'!B33&gt;0,'Deelnemers en Scores'!B33,"")</f>
         <v>5</v>
@@ -5025,7 +5026,7 @@
         <f>IF('Deelnemers en Scores'!H37=0,"",'Deelnemers en Scores'!H37)</f>
         <v/>
       </c>
-      <c r="I13" s="106"/>
+      <c r="I13" s="89"/>
       <c r="J13" s="18" t="str">
         <f>IF('Deelnemers en Scores'!I34=0,"",'Deelnemers en Scores'!I34)</f>
         <v/>
@@ -5042,52 +5043,52 @@
         <f>IF('Deelnemers en Scores'!I37=0,"",'Deelnemers en Scores'!I37)</f>
         <v/>
       </c>
-      <c r="N13" s="106"/>
+      <c r="N13" s="89"/>
       <c r="O13" s="19" t="str">
-        <f>IF(ISNUMBER(J13),E13+J13,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="P13" s="20" t="str">
-        <f>IF(ISNUMBER(K13),F13+K13,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q13" s="20" t="str">
-        <f>IF(ISNUMBER(L13),G13+L13,"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="R13" s="21" t="str">
-        <f>IF(ISNUMBER(M13),H13+M13,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S13" s="60">
-        <f>IF(COUNT(O13:R13)&lt;4,SUM(O13:R13),SUM(O13:R13)-MIN(O13:R13))</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T13" s="56">
-        <f>LARGE(O13:R13,1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U13" s="58">
-        <f>LARGE(O13:R13,2)</f>
-        <v>0</v>
-      </c>
-      <c r="V13" s="106"/>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V13" s="89"/>
       <c r="W13" s="59">
-        <f>S13+T13/10000+U13/10000000</f>
-        <v>0</v>
-      </c>
-      <c r="X13" s="99"/>
-      <c r="Y13" s="136" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="Z13" s="137" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X13" s="86"/>
+      <c r="Y13" s="114" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="Z13" s="115" t="str">
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
     <row r="14" spans="1:28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="96"/>
+      <c r="A14" s="83"/>
       <c r="B14" s="49">
         <f>IF('Deelnemers en Scores'!B39&gt;0,'Deelnemers en Scores'!B39,"")</f>
         <v>6</v>
@@ -5116,7 +5117,7 @@
         <f>IF('Deelnemers en Scores'!H43=0,"",'Deelnemers en Scores'!H43)</f>
         <v/>
       </c>
-      <c r="I14" s="106"/>
+      <c r="I14" s="89"/>
       <c r="J14" s="18" t="str">
         <f>IF('Deelnemers en Scores'!I40=0,"",'Deelnemers en Scores'!I40)</f>
         <v/>
@@ -5133,52 +5134,52 @@
         <f>IF('Deelnemers en Scores'!I43=0,"",'Deelnemers en Scores'!I43)</f>
         <v/>
       </c>
-      <c r="N14" s="106"/>
+      <c r="N14" s="89"/>
       <c r="O14" s="19" t="str">
-        <f>IF(ISNUMBER(J14),E14+J14,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="P14" s="20" t="str">
-        <f>IF(ISNUMBER(K14),F14+K14,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q14" s="20" t="str">
-        <f>IF(ISNUMBER(L14),G14+L14,"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="R14" s="21" t="str">
-        <f>IF(ISNUMBER(M14),H14+M14,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S14" s="60">
-        <f>IF(COUNT(O14:R14)&lt;4,SUM(O14:R14),SUM(O14:R14)-MIN(O14:R14))</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T14" s="56">
-        <f>LARGE(O14:R14,1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U14" s="58">
-        <f>LARGE(O14:R14,2)</f>
-        <v>0</v>
-      </c>
-      <c r="V14" s="106"/>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V14" s="89"/>
       <c r="W14" s="59">
-        <f>S14+T14/10000+U14/10000000</f>
-        <v>0</v>
-      </c>
-      <c r="X14" s="99"/>
-      <c r="Y14" s="136" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="Z14" s="137" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X14" s="86"/>
+      <c r="Y14" s="114" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="Z14" s="115" t="str">
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
     <row r="15" spans="1:28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="96"/>
+      <c r="A15" s="83"/>
       <c r="B15" s="49">
         <f>IF('Deelnemers en Scores'!B45&gt;0,'Deelnemers en Scores'!B45,"")</f>
         <v>7</v>
@@ -5207,7 +5208,7 @@
         <f>IF('Deelnemers en Scores'!H49=0,"",'Deelnemers en Scores'!H49)</f>
         <v/>
       </c>
-      <c r="I15" s="106"/>
+      <c r="I15" s="89"/>
       <c r="J15" s="18" t="str">
         <f>IF('Deelnemers en Scores'!I46=0,"",'Deelnemers en Scores'!I46)</f>
         <v/>
@@ -5224,52 +5225,52 @@
         <f>IF('Deelnemers en Scores'!I49=0,"",'Deelnemers en Scores'!I49)</f>
         <v/>
       </c>
-      <c r="N15" s="106"/>
+      <c r="N15" s="89"/>
       <c r="O15" s="19" t="str">
-        <f>IF(ISNUMBER(J15),E15+J15,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="P15" s="20" t="str">
-        <f>IF(ISNUMBER(K15),F15+K15,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q15" s="20" t="str">
-        <f>IF(ISNUMBER(L15),G15+L15,"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="R15" s="21" t="str">
-        <f>IF(ISNUMBER(M15),H15+M15,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S15" s="60">
-        <f>IF(COUNT(O15:R15)&lt;4,SUM(O15:R15),SUM(O15:R15)-MIN(O15:R15))</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T15" s="56">
-        <f>LARGE(O15:R15,1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U15" s="58">
-        <f>LARGE(O15:R15,2)</f>
-        <v>0</v>
-      </c>
-      <c r="V15" s="106"/>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V15" s="89"/>
       <c r="W15" s="59">
-        <f>S15+T15/10000+U15/10000000</f>
-        <v>0</v>
-      </c>
-      <c r="X15" s="99"/>
-      <c r="Y15" s="136" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="Z15" s="137" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X15" s="86"/>
+      <c r="Y15" s="114" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="Z15" s="115" t="str">
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
     <row r="16" spans="1:28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="96"/>
+      <c r="A16" s="83"/>
       <c r="B16" s="49">
         <f>IF('Deelnemers en Scores'!B51&gt;0,'Deelnemers en Scores'!B51,"")</f>
         <v>8</v>
@@ -5298,7 +5299,7 @@
         <f>IF('Deelnemers en Scores'!H55=0,"",'Deelnemers en Scores'!H55)</f>
         <v/>
       </c>
-      <c r="I16" s="106"/>
+      <c r="I16" s="89"/>
       <c r="J16" s="18" t="str">
         <f>IF('Deelnemers en Scores'!I52=0,"",'Deelnemers en Scores'!I52)</f>
         <v/>
@@ -5315,52 +5316,52 @@
         <f>IF('Deelnemers en Scores'!I55=0,"",'Deelnemers en Scores'!I55)</f>
         <v/>
       </c>
-      <c r="N16" s="106"/>
+      <c r="N16" s="89"/>
       <c r="O16" s="19" t="str">
-        <f>IF(ISNUMBER(J16),E16+J16,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="P16" s="20" t="str">
-        <f>IF(ISNUMBER(K16),F16+K16,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q16" s="20" t="str">
-        <f>IF(ISNUMBER(L16),G16+L16,"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="R16" s="21" t="str">
-        <f>IF(ISNUMBER(M16),H16+M16,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S16" s="60">
-        <f>IF(COUNT(O16:R16)&lt;4,SUM(O16:R16),SUM(O16:R16)-MIN(O16:R16))</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T16" s="56">
-        <f>LARGE(O16:R16,1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U16" s="58">
-        <f>LARGE(O16:R16,2)</f>
-        <v>0</v>
-      </c>
-      <c r="V16" s="106"/>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V16" s="89"/>
       <c r="W16" s="59">
-        <f>S16+T16/10000+U16/10000000</f>
-        <v>0</v>
-      </c>
-      <c r="X16" s="99"/>
-      <c r="Y16" s="136" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="Z16" s="137" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X16" s="86"/>
+      <c r="Y16" s="114" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="Z16" s="115" t="str">
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
     <row r="17" spans="1:26" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="96"/>
+      <c r="A17" s="83"/>
       <c r="B17" s="49">
         <f>IF('Deelnemers en Scores'!B57&gt;0,'Deelnemers en Scores'!B57,"")</f>
         <v>9</v>
@@ -5389,7 +5390,7 @@
         <f>IF('Deelnemers en Scores'!H61=0,"",'Deelnemers en Scores'!H61)</f>
         <v/>
       </c>
-      <c r="I17" s="106"/>
+      <c r="I17" s="89"/>
       <c r="J17" s="18" t="str">
         <f>IF('Deelnemers en Scores'!I58=0,"",'Deelnemers en Scores'!I58)</f>
         <v/>
@@ -5406,52 +5407,52 @@
         <f>IF('Deelnemers en Scores'!I61=0,"",'Deelnemers en Scores'!I61)</f>
         <v/>
       </c>
-      <c r="N17" s="106"/>
+      <c r="N17" s="89"/>
       <c r="O17" s="19" t="str">
-        <f>IF(ISNUMBER(J17),E17+J17,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="P17" s="20" t="str">
-        <f>IF(ISNUMBER(K17),F17+K17,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q17" s="20" t="str">
-        <f>IF(ISNUMBER(L17),G17+L17,"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="R17" s="21" t="str">
-        <f>IF(ISNUMBER(M17),H17+M17,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S17" s="60">
-        <f>IF(COUNT(O17:R17)&lt;4,SUM(O17:R17),SUM(O17:R17)-MIN(O17:R17))</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T17" s="56">
-        <f>LARGE(O17:R17,1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U17" s="58">
-        <f>LARGE(O17:R17,2)</f>
-        <v>0</v>
-      </c>
-      <c r="V17" s="106"/>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V17" s="89"/>
       <c r="W17" s="59">
-        <f>S17+T17/10000+U17/10000000</f>
-        <v>0</v>
-      </c>
-      <c r="X17" s="99"/>
-      <c r="Y17" s="136" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="Z17" s="137" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X17" s="86"/>
+      <c r="Y17" s="114" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="Z17" s="115" t="str">
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
     <row r="18" spans="1:26" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="96"/>
+      <c r="A18" s="83"/>
       <c r="B18" s="49">
         <f>IF('Deelnemers en Scores'!B63&gt;0,'Deelnemers en Scores'!B63,"")</f>
         <v>10</v>
@@ -5480,7 +5481,7 @@
         <f>IF('Deelnemers en Scores'!H67=0,"",'Deelnemers en Scores'!H67)</f>
         <v/>
       </c>
-      <c r="I18" s="106"/>
+      <c r="I18" s="89"/>
       <c r="J18" s="18" t="str">
         <f>IF('Deelnemers en Scores'!I64=0,"",'Deelnemers en Scores'!I64)</f>
         <v/>
@@ -5497,52 +5498,52 @@
         <f>IF('Deelnemers en Scores'!I67=0,"",'Deelnemers en Scores'!I67)</f>
         <v/>
       </c>
-      <c r="N18" s="106"/>
+      <c r="N18" s="89"/>
       <c r="O18" s="19" t="str">
-        <f>IF(ISNUMBER(J18),E18+J18,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="P18" s="20" t="str">
-        <f>IF(ISNUMBER(K18),F18+K18,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q18" s="20" t="str">
-        <f>IF(ISNUMBER(L18),G18+L18,"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="R18" s="21" t="str">
-        <f>IF(ISNUMBER(M18),H18+M18,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S18" s="60">
-        <f>IF(COUNT(O18:R18)&lt;4,SUM(O18:R18),SUM(O18:R18)-MIN(O18:R18))</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T18" s="56">
-        <f>LARGE(O18:R18,1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U18" s="58">
-        <f>LARGE(O18:R18,2)</f>
-        <v>0</v>
-      </c>
-      <c r="V18" s="106"/>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V18" s="89"/>
       <c r="W18" s="59">
-        <f>S18+T18/10000+U18/10000000</f>
-        <v>0</v>
-      </c>
-      <c r="X18" s="99"/>
-      <c r="Y18" s="136" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="Z18" s="137" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X18" s="86"/>
+      <c r="Y18" s="114" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="Z18" s="115" t="str">
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
     <row r="19" spans="1:26" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="96"/>
+      <c r="A19" s="83"/>
       <c r="B19" s="49">
         <f>IF('Deelnemers en Scores'!B69&gt;0,'Deelnemers en Scores'!B69,"")</f>
         <v>11</v>
@@ -5571,7 +5572,7 @@
         <f>IF('Deelnemers en Scores'!H73=0,"",'Deelnemers en Scores'!H73)</f>
         <v/>
       </c>
-      <c r="I19" s="106"/>
+      <c r="I19" s="89"/>
       <c r="J19" s="18" t="str">
         <f>IF('Deelnemers en Scores'!I70=0,"",'Deelnemers en Scores'!I70)</f>
         <v/>
@@ -5588,52 +5589,52 @@
         <f>IF('Deelnemers en Scores'!I73=0,"",'Deelnemers en Scores'!I73)</f>
         <v/>
       </c>
-      <c r="N19" s="106"/>
+      <c r="N19" s="89"/>
       <c r="O19" s="19" t="str">
-        <f>IF(ISNUMBER(J19),E19+J19,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="P19" s="20" t="str">
-        <f>IF(ISNUMBER(K19),F19+K19,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q19" s="20" t="str">
-        <f>IF(ISNUMBER(L19),G19+L19,"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="R19" s="21" t="str">
-        <f>IF(ISNUMBER(M19),H19+M19,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S19" s="60">
-        <f>IF(COUNT(O19:R19)&lt;4,SUM(O19:R19),SUM(O19:R19)-MIN(O19:R19))</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T19" s="56">
-        <f>LARGE(O19:R19,1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U19" s="58">
-        <f>LARGE(O19:R19,2)</f>
-        <v>0</v>
-      </c>
-      <c r="V19" s="106"/>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V19" s="89"/>
       <c r="W19" s="59">
-        <f>S19+T19/10000+U19/10000000</f>
-        <v>0</v>
-      </c>
-      <c r="X19" s="99"/>
-      <c r="Y19" s="136" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="Z19" s="137" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X19" s="86"/>
+      <c r="Y19" s="114" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="Z19" s="115" t="str">
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
     <row r="20" spans="1:26" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="96"/>
+      <c r="A20" s="83"/>
       <c r="B20" s="50">
         <f>IF('Deelnemers en Scores'!B75&gt;0,'Deelnemers en Scores'!B75,"")</f>
         <v>12</v>
@@ -5662,7 +5663,7 @@
         <f>IF('Deelnemers en Scores'!H79=0,"",'Deelnemers en Scores'!H79)</f>
         <v/>
       </c>
-      <c r="I20" s="107"/>
+      <c r="I20" s="90"/>
       <c r="J20" s="44" t="str">
         <f>IF('Deelnemers en Scores'!I76=0,"",'Deelnemers en Scores'!I76)</f>
         <v/>
@@ -5679,128 +5680,123 @@
         <f>IF('Deelnemers en Scores'!I79=0,"",'Deelnemers en Scores'!I79)</f>
         <v/>
       </c>
-      <c r="N20" s="107"/>
+      <c r="N20" s="90"/>
       <c r="O20" s="46" t="str">
-        <f>IF(ISNUMBER(J20),E20+J20,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="P20" s="47" t="str">
-        <f>IF(ISNUMBER(K20),F20+K20,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q20" s="47" t="str">
-        <f>IF(ISNUMBER(L20),G20+L20,"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="R20" s="48" t="str">
-        <f>IF(ISNUMBER(M20),H20+M20,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S20" s="60">
-        <f>IF(COUNT(O20:R20)&lt;4,SUM(O20:R20),SUM(O20:R20)-MIN(O20:R20))</f>
-        <v>0</v>
-      </c>
-      <c r="T20" s="108">
-        <f>LARGE(O20:R20,1)</f>
-        <v>0</v>
-      </c>
-      <c r="U20" s="109">
-        <f>LARGE(O20:R20,2)</f>
-        <v>0</v>
-      </c>
-      <c r="V20" s="107"/>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="T20" s="91">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="U20" s="92">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V20" s="90"/>
       <c r="W20" s="59">
-        <f>S20+T20/10000+U20/10000000</f>
-        <v>0</v>
-      </c>
-      <c r="X20" s="99"/>
-      <c r="Y20" s="136" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="Z20" s="137" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X20" s="86"/>
+      <c r="Y20" s="114" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="Z20" s="115" t="str">
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
     <row r="21" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="95"/>
-      <c r="B21" s="97"/>
-      <c r="C21" s="98"/>
-      <c r="D21" s="98"/>
-      <c r="E21" s="98"/>
-      <c r="F21" s="98"/>
-      <c r="G21" s="98"/>
-      <c r="H21" s="98"/>
-      <c r="I21" s="98"/>
-      <c r="J21" s="98"/>
-      <c r="K21" s="98"/>
-      <c r="L21" s="98"/>
-      <c r="M21" s="98"/>
-      <c r="N21" s="98"/>
-      <c r="O21" s="98"/>
-      <c r="P21" s="98"/>
-      <c r="Q21" s="98"/>
-      <c r="R21" s="98"/>
-      <c r="S21" s="98"/>
-      <c r="T21" s="98"/>
-      <c r="U21" s="98"/>
-      <c r="V21" s="98"/>
-      <c r="W21" s="98"/>
-      <c r="X21" s="95"/>
-      <c r="Y21" s="95"/>
+      <c r="A21" s="82"/>
+      <c r="B21" s="84"/>
+      <c r="C21" s="85"/>
+      <c r="D21" s="85"/>
+      <c r="E21" s="85"/>
+      <c r="F21" s="85"/>
+      <c r="G21" s="85"/>
+      <c r="H21" s="85"/>
+      <c r="I21" s="85"/>
+      <c r="J21" s="85"/>
+      <c r="K21" s="85"/>
+      <c r="L21" s="85"/>
+      <c r="M21" s="85"/>
+      <c r="N21" s="85"/>
+      <c r="O21" s="85"/>
+      <c r="P21" s="85"/>
+      <c r="Q21" s="85"/>
+      <c r="R21" s="85"/>
+      <c r="S21" s="85"/>
+      <c r="T21" s="85"/>
+      <c r="U21" s="85"/>
+      <c r="V21" s="85"/>
+      <c r="W21" s="85"/>
+      <c r="X21" s="82"/>
+      <c r="Y21" s="82"/>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.2"/>
     <row r="23" spans="1:26" ht="80.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K23" s="100" t="s">
+      <c r="K23" s="151" t="s">
         <v>87</v>
       </c>
-      <c r="L23" s="100"/>
-      <c r="M23" s="100"/>
-      <c r="N23" s="100"/>
-      <c r="O23" s="100"/>
-      <c r="P23" s="100"/>
-      <c r="Q23" s="100"/>
-      <c r="R23" s="100"/>
-      <c r="S23" s="100"/>
-      <c r="T23" s="100"/>
-      <c r="U23" s="100"/>
-      <c r="V23" s="100"/>
-      <c r="W23" s="100"/>
+      <c r="L23" s="151"/>
+      <c r="M23" s="151"/>
+      <c r="N23" s="151"/>
+      <c r="O23" s="151"/>
+      <c r="P23" s="151"/>
+      <c r="Q23" s="151"/>
+      <c r="R23" s="151"/>
+      <c r="S23" s="151"/>
+      <c r="T23" s="151"/>
+      <c r="U23" s="151"/>
+      <c r="V23" s="151"/>
+      <c r="W23" s="151"/>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="K24" s="101"/>
-      <c r="L24" s="101"/>
-      <c r="M24" s="101"/>
-      <c r="N24" s="101"/>
-      <c r="O24" s="101"/>
-      <c r="P24" s="101"/>
-      <c r="Q24" s="101"/>
-      <c r="R24" s="101"/>
-      <c r="S24" s="101"/>
-      <c r="T24" s="101"/>
-      <c r="U24" s="101"/>
-      <c r="V24" s="101"/>
-      <c r="W24" s="101"/>
+      <c r="K24" s="87"/>
+      <c r="L24" s="87"/>
+      <c r="M24" s="87"/>
+      <c r="N24" s="87"/>
+      <c r="O24" s="87"/>
+      <c r="P24" s="87"/>
+      <c r="Q24" s="87"/>
+      <c r="R24" s="87"/>
+      <c r="S24" s="87"/>
+      <c r="T24" s="87"/>
+      <c r="U24" s="87"/>
+      <c r="V24" s="87"/>
+      <c r="W24" s="87"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <autoFilter ref="B8:W20" xr:uid="{00000000-0001-0000-0200-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B9:W20">
-      <sortCondition descending="1" ref="W8:W20"/>
-    </sortState>
-  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B9:W20">
     <sortCondition descending="1" ref="W9"/>
   </sortState>
   <mergeCells count="7">
+    <mergeCell ref="K23:W23"/>
+    <mergeCell ref="T7:U7"/>
     <mergeCell ref="B2:W2"/>
     <mergeCell ref="P4:U4"/>
     <mergeCell ref="E7:H7"/>
     <mergeCell ref="J7:M7"/>
     <mergeCell ref="O7:R7"/>
-    <mergeCell ref="K23:W23"/>
-    <mergeCell ref="T7:U7"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.19685039370078741" right="0.39370078740157483" top="0.78740157480314965" bottom="0.39370078740157483" header="0.51181102362204722" footer="0.51181102362204722"/>

</xml_diff>

<commit_message>
Corrected filter to allow sorting results
</commit_message>
<xml_diff>
--- a/CompLaagBond/files/template-excel-bk-25m1pijl-teams.xlsx
+++ b/CompLaagBond/files/template-excel-bk-25m1pijl-teams.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects Ramon\Websites\NHB-applicaties\Excel programma's\BK excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CEFFB85-BB27-4BDA-B44B-8F48BB6AC986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0580AD-5A01-4386-8B41-5B690F0C22C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="18195" windowHeight="14025" tabRatio="546" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8640" yWindow="1095" windowWidth="18810" windowHeight="14025" tabRatio="546" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Uitleg" sheetId="16" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Uitslag" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Uitslag!$B$8:$W$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Uitslag!$W$8:$W$20</definedName>
     <definedName name="_Key1" hidden="1">#REF!</definedName>
     <definedName name="_Order1" hidden="1">255</definedName>
     <definedName name="_Sort" hidden="1">#REF!</definedName>
@@ -1668,6 +1668,9 @@
     <xf numFmtId="164" fontId="1" fillId="2" borderId="45" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1744,9 +1747,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2206,10 +2206,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:2" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="137" t="s">
+      <c r="A4" s="138" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="137"/>
+      <c r="B4" s="138"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
@@ -2340,7 +2340,7 @@
     <row r="34" spans="1:2" x14ac:dyDescent="0.2"/>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2"/>
     <row r="36" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="159" t="s">
+      <c r="A36" s="137" t="s">
         <v>97</v>
       </c>
     </row>
@@ -2389,17 +2389,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="24" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="138" t="str">
+      <c r="B1" s="139" t="str">
         <f>'Deelnemers en Scores'!B2</f>
         <v>BK 25m1pijl Teams, Klasse: komt hier</v>
       </c>
-      <c r="C1" s="139"/>
-      <c r="D1" s="139"/>
-      <c r="E1" s="139"/>
-      <c r="F1" s="139"/>
-      <c r="G1" s="139"/>
-      <c r="H1" s="139"/>
-      <c r="I1" s="140"/>
+      <c r="C1" s="140"/>
+      <c r="D1" s="140"/>
+      <c r="E1" s="140"/>
+      <c r="F1" s="140"/>
+      <c r="G1" s="140"/>
+      <c r="H1" s="140"/>
+      <c r="I1" s="141"/>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C2" s="10"/>
@@ -2560,18 +2560,18 @@
   <sheetData>
     <row r="1" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:11" ht="24" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="141" t="s">
+      <c r="B2" s="142" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="142"/>
-      <c r="D2" s="142"/>
-      <c r="E2" s="142"/>
-      <c r="F2" s="142"/>
-      <c r="G2" s="142"/>
-      <c r="H2" s="142"/>
-      <c r="I2" s="142"/>
-      <c r="J2" s="142"/>
-      <c r="K2" s="143"/>
+      <c r="C2" s="143"/>
+      <c r="D2" s="143"/>
+      <c r="E2" s="143"/>
+      <c r="F2" s="143"/>
+      <c r="G2" s="143"/>
+      <c r="H2" s="143"/>
+      <c r="I2" s="143"/>
+      <c r="J2" s="143"/>
+      <c r="K2" s="144"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B3" s="62"/>
@@ -2580,33 +2580,33 @@
       <c r="K3" s="67"/>
     </row>
     <row r="4" spans="2:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="145" t="s">
+      <c r="B4" s="146" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="146"/>
-      <c r="D4" s="146"/>
+      <c r="C4" s="147"/>
+      <c r="D4" s="147"/>
       <c r="E4" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="147" t="s">
+      <c r="F4" s="148" t="s">
         <v>45</v>
       </c>
       <c r="G4" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="148" t="s">
+      <c r="H4" s="149" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="148"/>
-      <c r="J4" s="148"/>
-      <c r="K4" s="149"/>
+      <c r="I4" s="149"/>
+      <c r="J4" s="149"/>
+      <c r="K4" s="150"/>
     </row>
     <row r="5" spans="2:11" ht="15" x14ac:dyDescent="0.2">
       <c r="B5" s="70"/>
       <c r="C5" s="71"/>
       <c r="D5" s="72"/>
       <c r="E5" s="71"/>
-      <c r="F5" s="147"/>
+      <c r="F5" s="148"/>
       <c r="G5" s="71"/>
       <c r="H5" s="73"/>
       <c r="I5" s="73"/>
@@ -2624,10 +2624,10 @@
       <c r="G6" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="H6" s="144" t="s">
+      <c r="H6" s="145" t="s">
         <v>48</v>
       </c>
-      <c r="I6" s="144"/>
+      <c r="I6" s="145"/>
       <c r="J6" s="75" t="s">
         <v>1</v>
       </c>
@@ -4390,31 +4390,31 @@
     </row>
     <row r="2" spans="1:28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="82"/>
-      <c r="B2" s="153" t="str">
+      <c r="B2" s="154" t="str">
         <f>'Deelnemers en Scores'!B2</f>
         <v>BK 25m1pijl Teams, Klasse: komt hier</v>
       </c>
-      <c r="C2" s="154"/>
-      <c r="D2" s="154"/>
-      <c r="E2" s="154"/>
-      <c r="F2" s="154"/>
-      <c r="G2" s="154"/>
-      <c r="H2" s="154"/>
-      <c r="I2" s="154"/>
-      <c r="J2" s="154"/>
-      <c r="K2" s="154"/>
-      <c r="L2" s="154"/>
-      <c r="M2" s="154"/>
-      <c r="N2" s="154"/>
-      <c r="O2" s="154"/>
-      <c r="P2" s="154"/>
-      <c r="Q2" s="154"/>
-      <c r="R2" s="154"/>
-      <c r="S2" s="154"/>
-      <c r="T2" s="154"/>
-      <c r="U2" s="154"/>
-      <c r="V2" s="154"/>
-      <c r="W2" s="155"/>
+      <c r="C2" s="155"/>
+      <c r="D2" s="155"/>
+      <c r="E2" s="155"/>
+      <c r="F2" s="155"/>
+      <c r="G2" s="155"/>
+      <c r="H2" s="155"/>
+      <c r="I2" s="155"/>
+      <c r="J2" s="155"/>
+      <c r="K2" s="155"/>
+      <c r="L2" s="155"/>
+      <c r="M2" s="155"/>
+      <c r="N2" s="155"/>
+      <c r="O2" s="155"/>
+      <c r="P2" s="155"/>
+      <c r="Q2" s="155"/>
+      <c r="R2" s="155"/>
+      <c r="S2" s="155"/>
+      <c r="T2" s="155"/>
+      <c r="U2" s="155"/>
+      <c r="V2" s="155"/>
+      <c r="W2" s="156"/>
       <c r="X2" s="82"/>
       <c r="Y2" s="82"/>
       <c r="Z2" s="82"/>
@@ -4465,15 +4465,15 @@
       <c r="O4" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="P4" s="156" t="str">
+      <c r="P4" s="157" t="str">
         <f>'Deelnemers en Scores'!H4</f>
         <v>yyyy-mm-dd</v>
       </c>
-      <c r="Q4" s="157"/>
-      <c r="R4" s="157"/>
-      <c r="S4" s="157"/>
-      <c r="T4" s="157"/>
-      <c r="U4" s="157"/>
+      <c r="Q4" s="158"/>
+      <c r="R4" s="158"/>
+      <c r="S4" s="158"/>
+      <c r="T4" s="158"/>
+      <c r="U4" s="158"/>
       <c r="V4" s="95"/>
       <c r="W4" s="96"/>
       <c r="X4" s="82"/>
@@ -4541,33 +4541,33 @@
       <c r="B7" s="97"/>
       <c r="C7" s="98"/>
       <c r="D7" s="99"/>
-      <c r="E7" s="151" t="s">
+      <c r="E7" s="152" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="158"/>
-      <c r="G7" s="158"/>
-      <c r="H7" s="158"/>
+      <c r="F7" s="159"/>
+      <c r="G7" s="159"/>
+      <c r="H7" s="159"/>
       <c r="I7" s="101"/>
-      <c r="J7" s="158" t="s">
+      <c r="J7" s="159" t="s">
         <v>36</v>
       </c>
-      <c r="K7" s="158"/>
-      <c r="L7" s="158"/>
-      <c r="M7" s="152"/>
+      <c r="K7" s="159"/>
+      <c r="L7" s="159"/>
+      <c r="M7" s="153"/>
       <c r="N7" s="100"/>
-      <c r="O7" s="151" t="s">
+      <c r="O7" s="152" t="s">
         <v>37</v>
       </c>
-      <c r="P7" s="158"/>
-      <c r="Q7" s="158"/>
-      <c r="R7" s="152"/>
+      <c r="P7" s="159"/>
+      <c r="Q7" s="159"/>
+      <c r="R7" s="153"/>
       <c r="S7" s="100" t="s">
         <v>88</v>
       </c>
-      <c r="T7" s="151" t="s">
+      <c r="T7" s="152" t="s">
         <v>87</v>
       </c>
-      <c r="U7" s="152"/>
+      <c r="U7" s="153"/>
       <c r="V7" s="101"/>
       <c r="W7" s="102" t="s">
         <v>86</v>
@@ -5763,21 +5763,21 @@
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.2"/>
     <row r="23" spans="1:26" ht="80.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K23" s="150" t="s">
+      <c r="K23" s="151" t="s">
         <v>84</v>
       </c>
-      <c r="L23" s="150"/>
-      <c r="M23" s="150"/>
-      <c r="N23" s="150"/>
-      <c r="O23" s="150"/>
-      <c r="P23" s="150"/>
-      <c r="Q23" s="150"/>
-      <c r="R23" s="150"/>
-      <c r="S23" s="150"/>
-      <c r="T23" s="150"/>
-      <c r="U23" s="150"/>
-      <c r="V23" s="150"/>
-      <c r="W23" s="150"/>
+      <c r="L23" s="151"/>
+      <c r="M23" s="151"/>
+      <c r="N23" s="151"/>
+      <c r="O23" s="151"/>
+      <c r="P23" s="151"/>
+      <c r="Q23" s="151"/>
+      <c r="R23" s="151"/>
+      <c r="S23" s="151"/>
+      <c r="T23" s="151"/>
+      <c r="U23" s="151"/>
+      <c r="V23" s="151"/>
+      <c r="W23" s="151"/>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="K24" s="87"/>
@@ -5796,7 +5796,7 @@
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <autoFilter ref="B8:W20" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
+  <autoFilter ref="W8:W20" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B9:W20">
     <sortCondition descending="1" ref="W9"/>
   </sortState>

</xml_diff>

<commit_message>
Pre-release v26, incl RK/BK teams Excel
</commit_message>
<xml_diff>
--- a/CompLaagBond/files/template-excel-bk-25m1pijl-teams.xlsx
+++ b/CompLaagBond/files/template-excel-bk-25m1pijl-teams.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects Ramon\Websites\NHB-applicaties\Excel programma's\BK excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0580AD-5A01-4386-8B41-5B690F0C22C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{753716A1-93CC-4D18-B712-B8C70D8C54CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8640" yWindow="1095" windowWidth="18810" windowHeight="14025" tabRatio="546" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="546" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Uitleg" sheetId="16" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Uitslag" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Uitslag!$W$8:$W$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Uitslag!$B$8:$AA$20</definedName>
     <definedName name="_Key1" hidden="1">#REF!</definedName>
     <definedName name="_Order1" hidden="1">255</definedName>
     <definedName name="_Sort" hidden="1">#REF!</definedName>
@@ -27,7 +27,7 @@
     <definedName name="FINALE_ZON">#REF!</definedName>
     <definedName name="PRINT_A">#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'Deelnemers en Scores'!$A$1:$L$81</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">Uitslag!$A$1:$Z$21</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">Uitslag!$A$1:$Z$23</definedName>
     <definedName name="PRINT_B">#REF!</definedName>
     <definedName name="PRINT_C">#REF!</definedName>
     <definedName name="PRINT_COMP_A">#REF!</definedName>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="100">
   <si>
     <t>Baan</t>
   </si>
@@ -382,28 +382,6 @@
     <t>Vereniging 123</t>
   </si>
   <si>
-    <r>
-      <t>Je hebt dit blad vooringevuld gekregen vanuit MijnHandboogsport met de laatste stand van zaken op moment van download. Aan het einde van het BK</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> moet het ingevulde bestand terug gestuurd worden</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> voor publicatie. Contactgegevens staan onderaan.</t>
-    </r>
-  </si>
-  <si>
     <t>Dit blad bevat alle gerechtigde deelnemers met hun gemiddelde + boogtype</t>
   </si>
   <si>
@@ -533,6 +511,34 @@
   </si>
   <si>
     <t>Contactgegevens</t>
+  </si>
+  <si>
+    <t>Sorteer mij</t>
+  </si>
+  <si>
+    <t>(hoog naar laag)</t>
+  </si>
+  <si>
+    <r>
+      <t>Je hebt dit blad vooringevuld gekregen vanuit MijnHandboogsport met de laatste stand van zaken op moment van download. Aan het einde van het BK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> moet het ingevulde bestand terug gestuurd worden</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> voor publicatie. De contactgegevens staan onderaan.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -660,7 +666,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -685,8 +691,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="51">
+  <borders count="54">
     <border>
       <left/>
       <right/>
@@ -1282,13 +1294,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="160">
+  <cellXfs count="163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1600,9 +1653,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1670,6 +1720,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="2" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1754,7 +1816,15 @@
     <cellStyle name="Normal 2" xfId="2" xr:uid="{2B25A250-A6E4-497C-B891-3A4CB2E3F5B3}"/>
     <cellStyle name="Standaard_team model" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -2201,19 +2271,19 @@
     <row r="1" spans="1:2" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:2" s="15" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:2" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="138" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" s="138"/>
+      <c r="A4" s="141" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="141"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2223,7 +2293,7 @@
     </row>
     <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2244,7 +2314,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -2291,12 +2361,12 @@
     </row>
     <row r="23" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2"/>
@@ -2314,44 +2384,44 @@
     </row>
     <row r="29" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B31" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B32" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2"/>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2"/>
     <row r="36" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="137" t="s">
-        <v>97</v>
+      <c r="A36" s="136" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B37" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B38" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2"/>
@@ -2389,17 +2459,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="24" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="139" t="str">
+      <c r="B1" s="142" t="str">
         <f>'Deelnemers en Scores'!B2</f>
         <v>BK 25m1pijl Teams, Klasse: komt hier</v>
       </c>
-      <c r="C1" s="140"/>
-      <c r="D1" s="140"/>
-      <c r="E1" s="140"/>
-      <c r="F1" s="140"/>
-      <c r="G1" s="140"/>
-      <c r="H1" s="140"/>
-      <c r="I1" s="141"/>
+      <c r="C1" s="143"/>
+      <c r="D1" s="143"/>
+      <c r="E1" s="143"/>
+      <c r="F1" s="143"/>
+      <c r="G1" s="143"/>
+      <c r="H1" s="143"/>
+      <c r="I1" s="144"/>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C2" s="10"/>
@@ -2419,12 +2489,12 @@
     </row>
     <row r="6" spans="2:9" ht="20.25" x14ac:dyDescent="0.2">
       <c r="D6" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="D7" s="35" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="14.25" x14ac:dyDescent="0.2">
@@ -2545,9 +2615,9 @@
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.109375" style="64" customWidth="1"/>
-    <col min="2" max="2" width="4.44140625" style="116" customWidth="1"/>
-    <col min="3" max="3" width="5.109375" style="116" customWidth="1"/>
-    <col min="4" max="4" width="29.33203125" style="116" customWidth="1"/>
+    <col min="2" max="2" width="4.44140625" style="115" customWidth="1"/>
+    <col min="3" max="3" width="5.109375" style="115" customWidth="1"/>
+    <col min="4" max="4" width="29.33203125" style="115" customWidth="1"/>
     <col min="5" max="5" width="7.77734375" style="64" customWidth="1"/>
     <col min="6" max="6" width="34.44140625" style="64" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" style="65" customWidth="1"/>
@@ -2560,18 +2630,18 @@
   <sheetData>
     <row r="1" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:11" ht="24" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="142" t="s">
-        <v>85</v>
-      </c>
-      <c r="C2" s="143"/>
-      <c r="D2" s="143"/>
-      <c r="E2" s="143"/>
-      <c r="F2" s="143"/>
-      <c r="G2" s="143"/>
-      <c r="H2" s="143"/>
-      <c r="I2" s="143"/>
-      <c r="J2" s="143"/>
-      <c r="K2" s="144"/>
+      <c r="B2" s="145" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="146"/>
+      <c r="D2" s="146"/>
+      <c r="E2" s="146"/>
+      <c r="F2" s="146"/>
+      <c r="G2" s="146"/>
+      <c r="H2" s="146"/>
+      <c r="I2" s="146"/>
+      <c r="J2" s="146"/>
+      <c r="K2" s="147"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B3" s="62"/>
@@ -2580,33 +2650,33 @@
       <c r="K3" s="67"/>
     </row>
     <row r="4" spans="2:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="146" t="s">
+      <c r="B4" s="149" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="147"/>
-      <c r="D4" s="147"/>
+      <c r="C4" s="150"/>
+      <c r="D4" s="150"/>
       <c r="E4" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="148" t="s">
+      <c r="F4" s="151" t="s">
         <v>45</v>
       </c>
       <c r="G4" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="149" t="s">
+      <c r="H4" s="152" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="149"/>
-      <c r="J4" s="149"/>
-      <c r="K4" s="150"/>
+      <c r="I4" s="152"/>
+      <c r="J4" s="152"/>
+      <c r="K4" s="153"/>
     </row>
     <row r="5" spans="2:11" ht="15" x14ac:dyDescent="0.2">
       <c r="B5" s="70"/>
       <c r="C5" s="71"/>
       <c r="D5" s="72"/>
       <c r="E5" s="71"/>
-      <c r="F5" s="148"/>
+      <c r="F5" s="151"/>
       <c r="G5" s="71"/>
       <c r="H5" s="73"/>
       <c r="I5" s="73"/>
@@ -2624,10 +2694,10 @@
       <c r="G6" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="H6" s="145" t="s">
+      <c r="H6" s="148" t="s">
         <v>48</v>
       </c>
-      <c r="I6" s="145"/>
+      <c r="I6" s="148"/>
       <c r="J6" s="75" t="s">
         <v>1</v>
       </c>
@@ -2668,44 +2738,44 @@
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B8" s="115"/>
-      <c r="E8" s="116"/>
-      <c r="F8" s="116"/>
-      <c r="G8" s="117"/>
-      <c r="H8" s="116"/>
-      <c r="I8" s="116"/>
-      <c r="J8" s="116"/>
-      <c r="K8" s="118"/>
+      <c r="B8" s="114"/>
+      <c r="E8" s="115"/>
+      <c r="F8" s="115"/>
+      <c r="G8" s="116"/>
+      <c r="H8" s="115"/>
+      <c r="I8" s="115"/>
+      <c r="J8" s="115"/>
+      <c r="K8" s="117"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B9" s="119">
+      <c r="B9" s="118">
         <v>1</v>
       </c>
-      <c r="C9" s="120">
+      <c r="C9" s="119">
         <v>100</v>
       </c>
-      <c r="D9" s="121" t="s">
+      <c r="D9" s="120" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="120"/>
-      <c r="F9" s="121" t="s">
+      <c r="E9" s="119"/>
+      <c r="F9" s="120" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="122">
+      <c r="G9" s="121">
         <v>888.8</v>
       </c>
-      <c r="H9" s="120"/>
-      <c r="I9" s="120"/>
-      <c r="J9" s="116"/>
-      <c r="K9" s="123">
+      <c r="H9" s="119"/>
+      <c r="I9" s="119"/>
+      <c r="J9" s="115"/>
+      <c r="K9" s="122">
         <f>IF(COUNTA(J10:J13)&lt;3,0,IF(COUNTA(J10:J13)=3,SUM(J10:J13),IF(SUM(J10:J13)&gt;0,SUM(J10:J13)-MINA(J10:J13),0)))</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="119"/>
-      <c r="C10" s="120"/>
-      <c r="D10" s="120"/>
+      <c r="B10" s="118"/>
+      <c r="C10" s="119"/>
+      <c r="D10" s="119"/>
       <c r="E10" s="8">
         <v>123456</v>
       </c>
@@ -2728,9 +2798,9 @@
       <c r="K10" s="67"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B11" s="119"/>
-      <c r="C11" s="120"/>
-      <c r="D11" s="120"/>
+      <c r="B11" s="118"/>
+      <c r="C11" s="119"/>
+      <c r="D11" s="119"/>
       <c r="E11" s="8">
         <v>123456</v>
       </c>
@@ -2753,9 +2823,9 @@
       <c r="K11" s="67"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B12" s="119"/>
-      <c r="C12" s="120"/>
-      <c r="D12" s="120"/>
+      <c r="B12" s="118"/>
+      <c r="C12" s="119"/>
+      <c r="D12" s="119"/>
       <c r="E12" s="8">
         <v>123456</v>
       </c>
@@ -2778,9 +2848,9 @@
       <c r="K12" s="67"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B13" s="119"/>
-      <c r="C13" s="120"/>
-      <c r="D13" s="120"/>
+      <c r="B13" s="118"/>
+      <c r="C13" s="119"/>
+      <c r="D13" s="119"/>
       <c r="E13" s="8">
         <v>123456</v>
       </c>
@@ -2803,45 +2873,45 @@
       <c r="K13" s="67"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B14" s="119"/>
-      <c r="C14" s="120"/>
-      <c r="D14" s="120"/>
-      <c r="E14" s="125"/>
-      <c r="F14" s="129"/>
-      <c r="G14" s="130"/>
-      <c r="H14" s="125"/>
-      <c r="I14" s="125"/>
+      <c r="B14" s="118"/>
+      <c r="C14" s="119"/>
+      <c r="D14" s="119"/>
+      <c r="E14" s="124"/>
+      <c r="F14" s="128"/>
+      <c r="G14" s="129"/>
+      <c r="H14" s="124"/>
+      <c r="I14" s="124"/>
       <c r="K14" s="67"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B15" s="119">
+      <c r="B15" s="118">
         <v>2</v>
       </c>
-      <c r="C15" s="120">
+      <c r="C15" s="119">
         <v>100</v>
       </c>
-      <c r="D15" s="121" t="s">
+      <c r="D15" s="120" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="120"/>
-      <c r="F15" s="121" t="s">
+      <c r="E15" s="119"/>
+      <c r="F15" s="120" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="122">
+      <c r="G15" s="121">
         <v>888.8</v>
       </c>
-      <c r="H15" s="125"/>
-      <c r="I15" s="125"/>
-      <c r="J15" s="116"/>
-      <c r="K15" s="123">
+      <c r="H15" s="124"/>
+      <c r="I15" s="124"/>
+      <c r="J15" s="115"/>
+      <c r="K15" s="122">
         <f>IF(COUNTA(J16:J19)&lt;3,0,IF(COUNTA(J16:J19)=3,SUM(J16:J19),IF(SUM(J16:J19)&gt;0,SUM(J16:J19)-MINA(J16:J19),0)))</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B16" s="119"/>
-      <c r="C16" s="120"/>
-      <c r="D16" s="120"/>
+      <c r="B16" s="118"/>
+      <c r="C16" s="119"/>
+      <c r="D16" s="119"/>
       <c r="E16" s="8">
         <v>123456</v>
       </c>
@@ -2864,9 +2934,9 @@
       <c r="K16" s="67"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B17" s="119"/>
-      <c r="C17" s="120"/>
-      <c r="D17" s="120"/>
+      <c r="B17" s="118"/>
+      <c r="C17" s="119"/>
+      <c r="D17" s="119"/>
       <c r="E17" s="8">
         <v>123456</v>
       </c>
@@ -2889,9 +2959,9 @@
       <c r="K17" s="67"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B18" s="119"/>
-      <c r="C18" s="120"/>
-      <c r="D18" s="120"/>
+      <c r="B18" s="118"/>
+      <c r="C18" s="119"/>
+      <c r="D18" s="119"/>
       <c r="E18" s="8">
         <v>123456</v>
       </c>
@@ -2914,9 +2984,9 @@
       <c r="K18" s="67"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B19" s="119"/>
-      <c r="C19" s="120"/>
-      <c r="D19" s="120"/>
+      <c r="B19" s="118"/>
+      <c r="C19" s="119"/>
+      <c r="D19" s="119"/>
       <c r="E19" s="8">
         <v>123456</v>
       </c>
@@ -2939,45 +3009,45 @@
       <c r="K19" s="67"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B20" s="119"/>
-      <c r="C20" s="120"/>
-      <c r="D20" s="120"/>
-      <c r="E20" s="125"/>
-      <c r="F20" s="129"/>
-      <c r="G20" s="130"/>
-      <c r="H20" s="125"/>
-      <c r="I20" s="125"/>
+      <c r="B20" s="118"/>
+      <c r="C20" s="119"/>
+      <c r="D20" s="119"/>
+      <c r="E20" s="124"/>
+      <c r="F20" s="128"/>
+      <c r="G20" s="129"/>
+      <c r="H20" s="124"/>
+      <c r="I20" s="124"/>
       <c r="K20" s="67"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B21" s="119">
+      <c r="B21" s="118">
         <v>3</v>
       </c>
-      <c r="C21" s="120">
+      <c r="C21" s="119">
         <v>100</v>
       </c>
-      <c r="D21" s="121" t="s">
+      <c r="D21" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="120"/>
-      <c r="F21" s="121" t="s">
+      <c r="E21" s="119"/>
+      <c r="F21" s="120" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="122">
+      <c r="G21" s="121">
         <v>888.8</v>
       </c>
-      <c r="H21" s="125"/>
-      <c r="I21" s="125"/>
-      <c r="J21" s="116"/>
-      <c r="K21" s="123">
+      <c r="H21" s="124"/>
+      <c r="I21" s="124"/>
+      <c r="J21" s="115"/>
+      <c r="K21" s="122">
         <f>IF(COUNTA(J22:J25)&lt;3,0,IF(COUNTA(J22:J25)=3,SUM(J22:J25),IF(SUM(J22:J25)&gt;0,SUM(J22:J25)-MINA(J22:J25),0)))</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B22" s="119"/>
-      <c r="C22" s="120"/>
-      <c r="D22" s="120"/>
+      <c r="B22" s="118"/>
+      <c r="C22" s="119"/>
+      <c r="D22" s="119"/>
       <c r="E22" s="8">
         <v>123456</v>
       </c>
@@ -3000,9 +3070,9 @@
       <c r="K22" s="67"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B23" s="119"/>
-      <c r="C23" s="120"/>
-      <c r="D23" s="120"/>
+      <c r="B23" s="118"/>
+      <c r="C23" s="119"/>
+      <c r="D23" s="119"/>
       <c r="E23" s="8">
         <v>123456</v>
       </c>
@@ -3025,9 +3095,9 @@
       <c r="K23" s="67"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B24" s="119"/>
-      <c r="C24" s="120"/>
-      <c r="D24" s="120"/>
+      <c r="B24" s="118"/>
+      <c r="C24" s="119"/>
+      <c r="D24" s="119"/>
       <c r="E24" s="8">
         <v>123456</v>
       </c>
@@ -3050,9 +3120,9 @@
       <c r="K24" s="67"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B25" s="119"/>
-      <c r="C25" s="120"/>
-      <c r="D25" s="120"/>
+      <c r="B25" s="118"/>
+      <c r="C25" s="119"/>
+      <c r="D25" s="119"/>
       <c r="E25" s="8">
         <v>123456</v>
       </c>
@@ -3075,45 +3145,45 @@
       <c r="K25" s="67"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B26" s="119"/>
-      <c r="C26" s="120"/>
-      <c r="D26" s="120"/>
-      <c r="E26" s="125"/>
-      <c r="F26" s="129"/>
-      <c r="G26" s="130"/>
-      <c r="H26" s="125"/>
-      <c r="I26" s="125"/>
+      <c r="B26" s="118"/>
+      <c r="C26" s="119"/>
+      <c r="D26" s="119"/>
+      <c r="E26" s="124"/>
+      <c r="F26" s="128"/>
+      <c r="G26" s="129"/>
+      <c r="H26" s="124"/>
+      <c r="I26" s="124"/>
       <c r="K26" s="67"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B27" s="119">
+      <c r="B27" s="118">
         <v>4</v>
       </c>
-      <c r="C27" s="120">
+      <c r="C27" s="119">
         <v>100</v>
       </c>
-      <c r="D27" s="121" t="s">
+      <c r="D27" s="120" t="s">
         <v>31</v>
       </c>
-      <c r="E27" s="120"/>
-      <c r="F27" s="121" t="s">
+      <c r="E27" s="119"/>
+      <c r="F27" s="120" t="s">
         <v>16</v>
       </c>
-      <c r="G27" s="122">
+      <c r="G27" s="121">
         <v>888.8</v>
       </c>
-      <c r="H27" s="125"/>
-      <c r="I27" s="125"/>
-      <c r="J27" s="116"/>
-      <c r="K27" s="123">
+      <c r="H27" s="124"/>
+      <c r="I27" s="124"/>
+      <c r="J27" s="115"/>
+      <c r="K27" s="122">
         <f>IF(COUNTA(J28:J31)&lt;3,0,IF(COUNTA(J28:J31)=3,SUM(J28:J31),IF(SUM(J28:J31)&gt;0,SUM(J28:J31)-MINA(J28:J31),0)))</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B28" s="119"/>
-      <c r="C28" s="120"/>
-      <c r="D28" s="120"/>
+      <c r="B28" s="118"/>
+      <c r="C28" s="119"/>
+      <c r="D28" s="119"/>
       <c r="E28" s="8">
         <v>123456</v>
       </c>
@@ -3136,9 +3206,9 @@
       <c r="K28" s="67"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B29" s="119"/>
-      <c r="C29" s="120"/>
-      <c r="D29" s="120"/>
+      <c r="B29" s="118"/>
+      <c r="C29" s="119"/>
+      <c r="D29" s="119"/>
       <c r="E29" s="8">
         <v>123456</v>
       </c>
@@ -3161,9 +3231,9 @@
       <c r="K29" s="67"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B30" s="119"/>
-      <c r="C30" s="120"/>
-      <c r="D30" s="120"/>
+      <c r="B30" s="118"/>
+      <c r="C30" s="119"/>
+      <c r="D30" s="119"/>
       <c r="E30" s="8">
         <v>123456</v>
       </c>
@@ -3186,9 +3256,9 @@
       <c r="K30" s="67"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B31" s="119"/>
-      <c r="C31" s="120"/>
-      <c r="D31" s="120"/>
+      <c r="B31" s="118"/>
+      <c r="C31" s="119"/>
+      <c r="D31" s="119"/>
       <c r="E31" s="8">
         <v>123456</v>
       </c>
@@ -3211,45 +3281,45 @@
       <c r="K31" s="67"/>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B32" s="119"/>
-      <c r="C32" s="120"/>
-      <c r="D32" s="120"/>
-      <c r="E32" s="125"/>
-      <c r="F32" s="129"/>
-      <c r="G32" s="130"/>
-      <c r="H32" s="125"/>
-      <c r="I32" s="125"/>
+      <c r="B32" s="118"/>
+      <c r="C32" s="119"/>
+      <c r="D32" s="119"/>
+      <c r="E32" s="124"/>
+      <c r="F32" s="128"/>
+      <c r="G32" s="129"/>
+      <c r="H32" s="124"/>
+      <c r="I32" s="124"/>
       <c r="K32" s="67"/>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B33" s="119">
+      <c r="B33" s="118">
         <v>5</v>
       </c>
-      <c r="C33" s="120">
+      <c r="C33" s="119">
         <v>100</v>
       </c>
-      <c r="D33" s="121" t="s">
+      <c r="D33" s="120" t="s">
         <v>32</v>
       </c>
-      <c r="E33" s="120"/>
-      <c r="F33" s="121" t="s">
+      <c r="E33" s="119"/>
+      <c r="F33" s="120" t="s">
         <v>33</v>
       </c>
-      <c r="G33" s="122">
+      <c r="G33" s="121">
         <v>888.8</v>
       </c>
-      <c r="H33" s="125"/>
-      <c r="I33" s="125"/>
-      <c r="J33" s="116"/>
-      <c r="K33" s="123">
+      <c r="H33" s="124"/>
+      <c r="I33" s="124"/>
+      <c r="J33" s="115"/>
+      <c r="K33" s="122">
         <f>IF(COUNTA(J34:J37)&lt;3,0,IF(COUNTA(J34:J37)=3,SUM(J34:J37),IF(SUM(J34:J37)&gt;0,SUM(J34:J37)-MINA(J34:J37),0)))</f>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B34" s="119"/>
-      <c r="C34" s="120"/>
-      <c r="D34" s="120"/>
+      <c r="B34" s="118"/>
+      <c r="C34" s="119"/>
+      <c r="D34" s="119"/>
       <c r="E34" s="8">
         <v>123456</v>
       </c>
@@ -3272,9 +3342,9 @@
       <c r="K34" s="67"/>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B35" s="119"/>
-      <c r="C35" s="120"/>
-      <c r="D35" s="120"/>
+      <c r="B35" s="118"/>
+      <c r="C35" s="119"/>
+      <c r="D35" s="119"/>
       <c r="E35" s="8">
         <v>123456</v>
       </c>
@@ -3297,9 +3367,9 @@
       <c r="K35" s="67"/>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B36" s="119"/>
-      <c r="C36" s="120"/>
-      <c r="D36" s="120"/>
+      <c r="B36" s="118"/>
+      <c r="C36" s="119"/>
+      <c r="D36" s="119"/>
       <c r="E36" s="8">
         <v>123456</v>
       </c>
@@ -3322,9 +3392,9 @@
       <c r="K36" s="67"/>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B37" s="119"/>
-      <c r="C37" s="120"/>
-      <c r="D37" s="120"/>
+      <c r="B37" s="118"/>
+      <c r="C37" s="119"/>
+      <c r="D37" s="119"/>
       <c r="E37" s="8">
         <v>123456</v>
       </c>
@@ -3347,45 +3417,45 @@
       <c r="K37" s="67"/>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B38" s="119"/>
-      <c r="C38" s="120"/>
-      <c r="D38" s="120"/>
-      <c r="E38" s="125"/>
-      <c r="F38" s="129"/>
-      <c r="G38" s="130"/>
-      <c r="H38" s="125"/>
-      <c r="I38" s="125"/>
+      <c r="B38" s="118"/>
+      <c r="C38" s="119"/>
+      <c r="D38" s="119"/>
+      <c r="E38" s="124"/>
+      <c r="F38" s="128"/>
+      <c r="G38" s="129"/>
+      <c r="H38" s="124"/>
+      <c r="I38" s="124"/>
       <c r="K38" s="67"/>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B39" s="119">
+      <c r="B39" s="118">
         <v>6</v>
       </c>
-      <c r="C39" s="120">
+      <c r="C39" s="119">
         <v>100</v>
       </c>
-      <c r="D39" s="121" t="s">
+      <c r="D39" s="120" t="s">
         <v>29</v>
       </c>
-      <c r="E39" s="120"/>
-      <c r="F39" s="121" t="s">
+      <c r="E39" s="119"/>
+      <c r="F39" s="120" t="s">
         <v>30</v>
       </c>
-      <c r="G39" s="122">
+      <c r="G39" s="121">
         <v>888.8</v>
       </c>
-      <c r="H39" s="125"/>
-      <c r="I39" s="125"/>
-      <c r="J39" s="116"/>
-      <c r="K39" s="123">
+      <c r="H39" s="124"/>
+      <c r="I39" s="124"/>
+      <c r="J39" s="115"/>
+      <c r="K39" s="122">
         <f>IF(COUNTA(J40:J43)&lt;3,0,IF(COUNTA(J40:J43)=3,SUM(J40:J43),IF(SUM(J40:J43)&gt;0,SUM(J40:J43)-MINA(J40:J43),0)))</f>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B40" s="119"/>
-      <c r="C40" s="120"/>
-      <c r="D40" s="120"/>
+      <c r="B40" s="118"/>
+      <c r="C40" s="119"/>
+      <c r="D40" s="119"/>
       <c r="E40" s="8">
         <v>123456</v>
       </c>
@@ -3408,9 +3478,9 @@
       <c r="K40" s="67"/>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B41" s="119"/>
-      <c r="C41" s="120"/>
-      <c r="D41" s="120"/>
+      <c r="B41" s="118"/>
+      <c r="C41" s="119"/>
+      <c r="D41" s="119"/>
       <c r="E41" s="8">
         <v>123456</v>
       </c>
@@ -3433,9 +3503,9 @@
       <c r="K41" s="67"/>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B42" s="119"/>
-      <c r="C42" s="120"/>
-      <c r="D42" s="120"/>
+      <c r="B42" s="118"/>
+      <c r="C42" s="119"/>
+      <c r="D42" s="119"/>
       <c r="E42" s="8">
         <v>123456</v>
       </c>
@@ -3458,9 +3528,9 @@
       <c r="K42" s="67"/>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B43" s="119"/>
-      <c r="C43" s="120"/>
-      <c r="D43" s="120"/>
+      <c r="B43" s="118"/>
+      <c r="C43" s="119"/>
+      <c r="D43" s="119"/>
       <c r="E43" s="8">
         <v>123456</v>
       </c>
@@ -3483,45 +3553,45 @@
       <c r="K43" s="67"/>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B44" s="119"/>
-      <c r="C44" s="120"/>
-      <c r="D44" s="120"/>
-      <c r="E44" s="125"/>
-      <c r="F44" s="129"/>
-      <c r="G44" s="130"/>
-      <c r="H44" s="125"/>
-      <c r="I44" s="125"/>
+      <c r="B44" s="118"/>
+      <c r="C44" s="119"/>
+      <c r="D44" s="119"/>
+      <c r="E44" s="124"/>
+      <c r="F44" s="128"/>
+      <c r="G44" s="129"/>
+      <c r="H44" s="124"/>
+      <c r="I44" s="124"/>
       <c r="K44" s="67"/>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B45" s="119">
+      <c r="B45" s="118">
         <v>7</v>
       </c>
-      <c r="C45" s="120">
+      <c r="C45" s="119">
         <v>100</v>
       </c>
-      <c r="D45" s="121" t="s">
+      <c r="D45" s="120" t="s">
         <v>27</v>
       </c>
-      <c r="E45" s="120"/>
-      <c r="F45" s="121" t="s">
+      <c r="E45" s="119"/>
+      <c r="F45" s="120" t="s">
         <v>28</v>
       </c>
-      <c r="G45" s="122">
+      <c r="G45" s="121">
         <v>888.8</v>
       </c>
-      <c r="H45" s="125"/>
-      <c r="I45" s="125"/>
-      <c r="J45" s="116"/>
-      <c r="K45" s="123">
+      <c r="H45" s="124"/>
+      <c r="I45" s="124"/>
+      <c r="J45" s="115"/>
+      <c r="K45" s="122">
         <f>IF(COUNTA(J46:J49)&lt;3,0,IF(COUNTA(J46:J49)=3,SUM(J46:J49),IF(SUM(J46:J49)&gt;0,SUM(J46:J49)-MINA(J46:J49),0)))</f>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B46" s="119"/>
-      <c r="C46" s="120"/>
-      <c r="D46" s="120"/>
+      <c r="B46" s="118"/>
+      <c r="C46" s="119"/>
+      <c r="D46" s="119"/>
       <c r="E46" s="8">
         <v>123456</v>
       </c>
@@ -3544,9 +3614,9 @@
       <c r="K46" s="67"/>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B47" s="119"/>
-      <c r="C47" s="120"/>
-      <c r="D47" s="120"/>
+      <c r="B47" s="118"/>
+      <c r="C47" s="119"/>
+      <c r="D47" s="119"/>
       <c r="E47" s="8">
         <v>123456</v>
       </c>
@@ -3569,9 +3639,9 @@
       <c r="K47" s="67"/>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B48" s="119"/>
-      <c r="C48" s="120"/>
-      <c r="D48" s="120"/>
+      <c r="B48" s="118"/>
+      <c r="C48" s="119"/>
+      <c r="D48" s="119"/>
       <c r="E48" s="8">
         <v>123456</v>
       </c>
@@ -3594,9 +3664,9 @@
       <c r="K48" s="67"/>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B49" s="119"/>
-      <c r="C49" s="120"/>
-      <c r="D49" s="120"/>
+      <c r="B49" s="118"/>
+      <c r="C49" s="119"/>
+      <c r="D49" s="119"/>
       <c r="E49" s="8">
         <v>123456</v>
       </c>
@@ -3619,45 +3689,45 @@
       <c r="K49" s="67"/>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B50" s="119"/>
-      <c r="C50" s="120"/>
-      <c r="D50" s="120"/>
-      <c r="E50" s="125"/>
-      <c r="F50" s="129"/>
-      <c r="G50" s="130"/>
-      <c r="H50" s="125"/>
-      <c r="I50" s="125"/>
+      <c r="B50" s="118"/>
+      <c r="C50" s="119"/>
+      <c r="D50" s="119"/>
+      <c r="E50" s="124"/>
+      <c r="F50" s="128"/>
+      <c r="G50" s="129"/>
+      <c r="H50" s="124"/>
+      <c r="I50" s="124"/>
       <c r="K50" s="67"/>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B51" s="119">
+      <c r="B51" s="118">
         <v>8</v>
       </c>
-      <c r="C51" s="120">
+      <c r="C51" s="119">
         <v>100</v>
       </c>
-      <c r="D51" s="121" t="s">
+      <c r="D51" s="120" t="s">
         <v>25</v>
       </c>
-      <c r="E51" s="120"/>
-      <c r="F51" s="121" t="s">
+      <c r="E51" s="119"/>
+      <c r="F51" s="120" t="s">
         <v>26</v>
       </c>
-      <c r="G51" s="122">
+      <c r="G51" s="121">
         <v>888.8</v>
       </c>
-      <c r="H51" s="125"/>
-      <c r="I51" s="125"/>
-      <c r="J51" s="116"/>
-      <c r="K51" s="123">
+      <c r="H51" s="124"/>
+      <c r="I51" s="124"/>
+      <c r="J51" s="115"/>
+      <c r="K51" s="122">
         <f>IF(COUNTA(J52:J55)&lt;3,0,IF(COUNTA(J52:J55)=3,SUM(J52:J55),IF(SUM(J52:J55)&gt;0,SUM(J52:J55)-MINA(J52:J55),0)))</f>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B52" s="119"/>
-      <c r="C52" s="120"/>
-      <c r="D52" s="120"/>
+      <c r="B52" s="118"/>
+      <c r="C52" s="119"/>
+      <c r="D52" s="119"/>
       <c r="E52" s="8">
         <v>123456</v>
       </c>
@@ -3680,9 +3750,9 @@
       <c r="K52" s="67"/>
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B53" s="119"/>
-      <c r="C53" s="120"/>
-      <c r="D53" s="120"/>
+      <c r="B53" s="118"/>
+      <c r="C53" s="119"/>
+      <c r="D53" s="119"/>
       <c r="E53" s="8">
         <v>123456</v>
       </c>
@@ -3705,9 +3775,9 @@
       <c r="K53" s="67"/>
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B54" s="119"/>
-      <c r="C54" s="120"/>
-      <c r="D54" s="120"/>
+      <c r="B54" s="118"/>
+      <c r="C54" s="119"/>
+      <c r="D54" s="119"/>
       <c r="E54" s="8">
         <v>123456</v>
       </c>
@@ -3730,9 +3800,9 @@
       <c r="K54" s="67"/>
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B55" s="119"/>
-      <c r="C55" s="120"/>
-      <c r="D55" s="120"/>
+      <c r="B55" s="118"/>
+      <c r="C55" s="119"/>
+      <c r="D55" s="119"/>
       <c r="E55" s="8">
         <v>123456</v>
       </c>
@@ -3755,45 +3825,45 @@
       <c r="K55" s="67"/>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B56" s="119"/>
-      <c r="C56" s="120"/>
-      <c r="D56" s="120"/>
-      <c r="E56" s="125"/>
-      <c r="F56" s="129"/>
-      <c r="G56" s="130"/>
-      <c r="H56" s="125"/>
-      <c r="I56" s="125"/>
+      <c r="B56" s="118"/>
+      <c r="C56" s="119"/>
+      <c r="D56" s="119"/>
+      <c r="E56" s="124"/>
+      <c r="F56" s="128"/>
+      <c r="G56" s="129"/>
+      <c r="H56" s="124"/>
+      <c r="I56" s="124"/>
       <c r="K56" s="67"/>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B57" s="119">
+      <c r="B57" s="118">
         <v>9</v>
       </c>
-      <c r="C57" s="120">
+      <c r="C57" s="119">
         <v>100</v>
       </c>
-      <c r="D57" s="121" t="s">
+      <c r="D57" s="120" t="s">
         <v>23</v>
       </c>
-      <c r="E57" s="120"/>
-      <c r="F57" s="121" t="s">
+      <c r="E57" s="119"/>
+      <c r="F57" s="120" t="s">
         <v>24</v>
       </c>
-      <c r="G57" s="122">
+      <c r="G57" s="121">
         <v>888.8</v>
       </c>
-      <c r="H57" s="125"/>
-      <c r="I57" s="125"/>
-      <c r="J57" s="116"/>
-      <c r="K57" s="123">
+      <c r="H57" s="124"/>
+      <c r="I57" s="124"/>
+      <c r="J57" s="115"/>
+      <c r="K57" s="122">
         <f>IF(COUNTA(J58:J61)&lt;3,0,IF(COUNTA(J58:J61)=3,SUM(J58:J61),IF(SUM(J58:J61)&gt;0,SUM(J58:J61)-MINA(J58:J61),0)))</f>
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B58" s="119"/>
-      <c r="C58" s="120"/>
-      <c r="D58" s="120"/>
+      <c r="B58" s="118"/>
+      <c r="C58" s="119"/>
+      <c r="D58" s="119"/>
       <c r="E58" s="8">
         <v>123456</v>
       </c>
@@ -3816,9 +3886,9 @@
       <c r="K58" s="67"/>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B59" s="119"/>
-      <c r="C59" s="120"/>
-      <c r="D59" s="120"/>
+      <c r="B59" s="118"/>
+      <c r="C59" s="119"/>
+      <c r="D59" s="119"/>
       <c r="E59" s="8">
         <v>123456</v>
       </c>
@@ -3841,9 +3911,9 @@
       <c r="K59" s="67"/>
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B60" s="119"/>
-      <c r="C60" s="120"/>
-      <c r="D60" s="120"/>
+      <c r="B60" s="118"/>
+      <c r="C60" s="119"/>
+      <c r="D60" s="119"/>
       <c r="E60" s="8">
         <v>123456</v>
       </c>
@@ -3866,9 +3936,9 @@
       <c r="K60" s="67"/>
     </row>
     <row r="61" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B61" s="119"/>
-      <c r="C61" s="120"/>
-      <c r="D61" s="120"/>
+      <c r="B61" s="118"/>
+      <c r="C61" s="119"/>
+      <c r="D61" s="119"/>
       <c r="E61" s="8">
         <v>123456</v>
       </c>
@@ -3891,46 +3961,46 @@
       <c r="K61" s="67"/>
     </row>
     <row r="62" spans="2:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="B62" s="126"/>
+      <c r="B62" s="125"/>
       <c r="C62" s="82"/>
       <c r="D62" s="82"/>
       <c r="E62" s="82"/>
       <c r="F62" s="82"/>
-      <c r="G62" s="127"/>
-      <c r="H62" s="125"/>
-      <c r="I62" s="125"/>
+      <c r="G62" s="126"/>
+      <c r="H62" s="124"/>
+      <c r="I62" s="124"/>
       <c r="J62" s="82"/>
-      <c r="K62" s="128"/>
+      <c r="K62" s="127"/>
     </row>
     <row r="63" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B63" s="119">
+      <c r="B63" s="118">
         <v>10</v>
       </c>
-      <c r="C63" s="120">
+      <c r="C63" s="119">
         <v>100</v>
       </c>
-      <c r="D63" s="121" t="s">
+      <c r="D63" s="120" t="s">
         <v>21</v>
       </c>
-      <c r="E63" s="120"/>
-      <c r="F63" s="121" t="s">
+      <c r="E63" s="119"/>
+      <c r="F63" s="120" t="s">
         <v>22</v>
       </c>
-      <c r="G63" s="122">
+      <c r="G63" s="121">
         <v>888.8</v>
       </c>
-      <c r="H63" s="125"/>
-      <c r="I63" s="125"/>
-      <c r="J63" s="116"/>
-      <c r="K63" s="123">
+      <c r="H63" s="124"/>
+      <c r="I63" s="124"/>
+      <c r="J63" s="115"/>
+      <c r="K63" s="122">
         <f>IF(COUNTA(J64:J67)&lt;3,0,IF(COUNTA(J64:J67)=3,SUM(J64:J67),IF(SUM(J64:J67)&gt;0,SUM(J64:J67)-MINA(J64:J67),0)))</f>
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B64" s="119"/>
-      <c r="C64" s="120"/>
-      <c r="D64" s="120"/>
+      <c r="B64" s="118"/>
+      <c r="C64" s="119"/>
+      <c r="D64" s="119"/>
       <c r="E64" s="8">
         <v>123456</v>
       </c>
@@ -3953,9 +4023,9 @@
       <c r="K64" s="67"/>
     </row>
     <row r="65" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B65" s="119"/>
-      <c r="C65" s="120"/>
-      <c r="D65" s="120"/>
+      <c r="B65" s="118"/>
+      <c r="C65" s="119"/>
+      <c r="D65" s="119"/>
       <c r="E65" s="8">
         <v>123456</v>
       </c>
@@ -3978,9 +4048,9 @@
       <c r="K65" s="67"/>
     </row>
     <row r="66" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B66" s="119"/>
-      <c r="C66" s="120"/>
-      <c r="D66" s="120"/>
+      <c r="B66" s="118"/>
+      <c r="C66" s="119"/>
+      <c r="D66" s="119"/>
       <c r="E66" s="8">
         <v>123456</v>
       </c>
@@ -4003,9 +4073,9 @@
       <c r="K66" s="67"/>
     </row>
     <row r="67" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B67" s="119"/>
-      <c r="C67" s="120"/>
-      <c r="D67" s="120"/>
+      <c r="B67" s="118"/>
+      <c r="C67" s="119"/>
+      <c r="D67" s="119"/>
       <c r="E67" s="8">
         <v>123456</v>
       </c>
@@ -4028,40 +4098,40 @@
       <c r="K67" s="67"/>
     </row>
     <row r="68" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B68" s="115"/>
-      <c r="H68" s="125"/>
-      <c r="I68" s="125"/>
+      <c r="B68" s="114"/>
+      <c r="H68" s="124"/>
+      <c r="I68" s="124"/>
       <c r="K68" s="67"/>
     </row>
     <row r="69" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B69" s="119">
+      <c r="B69" s="118">
         <v>11</v>
       </c>
-      <c r="C69" s="120">
+      <c r="C69" s="119">
         <v>100</v>
       </c>
-      <c r="D69" s="121" t="s">
+      <c r="D69" s="120" t="s">
         <v>20</v>
       </c>
-      <c r="E69" s="120"/>
-      <c r="F69" s="121" t="s">
+      <c r="E69" s="119"/>
+      <c r="F69" s="120" t="s">
         <v>19</v>
       </c>
-      <c r="G69" s="122">
+      <c r="G69" s="121">
         <v>888.8</v>
       </c>
-      <c r="H69" s="125"/>
-      <c r="I69" s="125"/>
-      <c r="J69" s="116"/>
-      <c r="K69" s="123">
+      <c r="H69" s="124"/>
+      <c r="I69" s="124"/>
+      <c r="J69" s="115"/>
+      <c r="K69" s="122">
         <f>IF(COUNTA(J70:J73)&lt;3,0,IF(COUNTA(J70:J73)=3,SUM(J70:J73),IF(SUM(J70:J73)&gt;0,SUM(J70:J73)-MINA(J70:J73),0)))</f>
         <v>0</v>
       </c>
     </row>
     <row r="70" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B70" s="119"/>
-      <c r="C70" s="120"/>
-      <c r="D70" s="120"/>
+      <c r="B70" s="118"/>
+      <c r="C70" s="119"/>
+      <c r="D70" s="119"/>
       <c r="E70" s="8">
         <v>123456</v>
       </c>
@@ -4084,9 +4154,9 @@
       <c r="K70" s="67"/>
     </row>
     <row r="71" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B71" s="119"/>
-      <c r="C71" s="120"/>
-      <c r="D71" s="120"/>
+      <c r="B71" s="118"/>
+      <c r="C71" s="119"/>
+      <c r="D71" s="119"/>
       <c r="E71" s="8">
         <v>123456</v>
       </c>
@@ -4109,9 +4179,9 @@
       <c r="K71" s="67"/>
     </row>
     <row r="72" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B72" s="119"/>
-      <c r="C72" s="120"/>
-      <c r="D72" s="120"/>
+      <c r="B72" s="118"/>
+      <c r="C72" s="119"/>
+      <c r="D72" s="119"/>
       <c r="E72" s="8">
         <v>123456</v>
       </c>
@@ -4134,9 +4204,9 @@
       <c r="K72" s="67"/>
     </row>
     <row r="73" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B73" s="119"/>
-      <c r="C73" s="120"/>
-      <c r="D73" s="120"/>
+      <c r="B73" s="118"/>
+      <c r="C73" s="119"/>
+      <c r="D73" s="119"/>
       <c r="E73" s="8">
         <v>123456</v>
       </c>
@@ -4159,40 +4229,40 @@
       <c r="K73" s="67"/>
     </row>
     <row r="74" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B74" s="115"/>
-      <c r="H74" s="125"/>
-      <c r="I74" s="125"/>
+      <c r="B74" s="114"/>
+      <c r="H74" s="124"/>
+      <c r="I74" s="124"/>
       <c r="K74" s="67"/>
     </row>
     <row r="75" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B75" s="119">
+      <c r="B75" s="118">
         <v>12</v>
       </c>
-      <c r="C75" s="120">
+      <c r="C75" s="119">
         <v>100</v>
       </c>
-      <c r="D75" s="121" t="s">
+      <c r="D75" s="120" t="s">
         <v>17</v>
       </c>
-      <c r="E75" s="120"/>
-      <c r="F75" s="121" t="s">
+      <c r="E75" s="119"/>
+      <c r="F75" s="120" t="s">
         <v>18</v>
       </c>
-      <c r="G75" s="122">
+      <c r="G75" s="121">
         <v>888.8</v>
       </c>
-      <c r="H75" s="125"/>
-      <c r="I75" s="125"/>
-      <c r="J75" s="116"/>
-      <c r="K75" s="123">
+      <c r="H75" s="124"/>
+      <c r="I75" s="124"/>
+      <c r="J75" s="115"/>
+      <c r="K75" s="122">
         <f>IF(COUNTA(J76:J79)&lt;3,0,IF(COUNTA(J76:J79)=3,SUM(J76:J79),IF(SUM(J76:J79)&gt;0,SUM(J76:J79)-MINA(J76:J79),0)))</f>
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B76" s="119"/>
-      <c r="C76" s="120"/>
-      <c r="D76" s="120"/>
+      <c r="B76" s="118"/>
+      <c r="C76" s="119"/>
+      <c r="D76" s="119"/>
       <c r="E76" s="8">
         <v>123456</v>
       </c>
@@ -4215,9 +4285,9 @@
       <c r="K76" s="67"/>
     </row>
     <row r="77" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B77" s="119"/>
-      <c r="C77" s="120"/>
-      <c r="D77" s="120"/>
+      <c r="B77" s="118"/>
+      <c r="C77" s="119"/>
+      <c r="D77" s="119"/>
       <c r="E77" s="8">
         <v>123456</v>
       </c>
@@ -4240,9 +4310,9 @@
       <c r="K77" s="67"/>
     </row>
     <row r="78" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B78" s="119"/>
-      <c r="C78" s="120"/>
-      <c r="D78" s="120"/>
+      <c r="B78" s="118"/>
+      <c r="C78" s="119"/>
+      <c r="D78" s="119"/>
       <c r="E78" s="8">
         <v>123456</v>
       </c>
@@ -4265,9 +4335,9 @@
       <c r="K78" s="67"/>
     </row>
     <row r="79" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B79" s="119"/>
-      <c r="C79" s="120"/>
-      <c r="D79" s="120"/>
+      <c r="B79" s="118"/>
+      <c r="C79" s="119"/>
+      <c r="D79" s="119"/>
       <c r="E79" s="8">
         <v>123456</v>
       </c>
@@ -4290,20 +4360,20 @@
       <c r="K79" s="67"/>
     </row>
     <row r="80" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="133"/>
-      <c r="C80" s="134"/>
-      <c r="D80" s="134"/>
-      <c r="E80" s="135"/>
-      <c r="F80" s="135"/>
-      <c r="G80" s="136"/>
-      <c r="H80" s="131"/>
-      <c r="I80" s="131"/>
-      <c r="J80" s="131"/>
-      <c r="K80" s="132"/>
+      <c r="B80" s="132"/>
+      <c r="C80" s="133"/>
+      <c r="D80" s="133"/>
+      <c r="E80" s="134"/>
+      <c r="F80" s="134"/>
+      <c r="G80" s="135"/>
+      <c r="H80" s="130"/>
+      <c r="I80" s="130"/>
+      <c r="J80" s="130"/>
+      <c r="K80" s="131"/>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.2"/>
     <row r="82" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B82" s="124" t="s">
+      <c r="B82" s="123" t="s">
         <v>47</v>
       </c>
     </row>
@@ -4338,7 +4408,7 @@
   <sheetPr transitionEvaluation="1" codeName="Blad3">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AB24"/>
+  <dimension ref="A1:AC24"/>
   <sheetViews>
     <sheetView defaultGridColor="0" colorId="22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
@@ -4355,12 +4425,13 @@
     <col min="22" max="22" width="2.109375" style="82" customWidth="1"/>
     <col min="23" max="23" width="10.33203125" style="82" customWidth="1"/>
     <col min="24" max="24" width="0.88671875" style="82" customWidth="1"/>
-    <col min="25" max="25" width="3.44140625" style="82" customWidth="1"/>
-    <col min="26" max="26" width="3" style="82" customWidth="1"/>
-    <col min="27" max="16384" width="9.77734375" style="82" hidden="1"/>
+    <col min="25" max="25" width="3.44140625" style="82" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="5" style="82" customWidth="1"/>
+    <col min="27" max="27" width="17.44140625" style="82" customWidth="1"/>
+    <col min="28" max="16384" width="9.77734375" style="82" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="82"/>
       <c r="B1" s="83"/>
       <c r="C1" s="82"/>
@@ -4387,39 +4458,41 @@
       <c r="X1" s="82"/>
       <c r="Y1" s="82"/>
       <c r="Z1" s="82"/>
-    </row>
-    <row r="2" spans="1:28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA1" s="82"/>
+    </row>
+    <row r="2" spans="1:29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="82"/>
-      <c r="B2" s="154" t="str">
+      <c r="B2" s="157" t="str">
         <f>'Deelnemers en Scores'!B2</f>
         <v>BK 25m1pijl Teams, Klasse: komt hier</v>
       </c>
-      <c r="C2" s="155"/>
-      <c r="D2" s="155"/>
-      <c r="E2" s="155"/>
-      <c r="F2" s="155"/>
-      <c r="G2" s="155"/>
-      <c r="H2" s="155"/>
-      <c r="I2" s="155"/>
-      <c r="J2" s="155"/>
-      <c r="K2" s="155"/>
-      <c r="L2" s="155"/>
-      <c r="M2" s="155"/>
-      <c r="N2" s="155"/>
-      <c r="O2" s="155"/>
-      <c r="P2" s="155"/>
-      <c r="Q2" s="155"/>
-      <c r="R2" s="155"/>
-      <c r="S2" s="155"/>
-      <c r="T2" s="155"/>
-      <c r="U2" s="155"/>
-      <c r="V2" s="155"/>
-      <c r="W2" s="156"/>
+      <c r="C2" s="158"/>
+      <c r="D2" s="158"/>
+      <c r="E2" s="158"/>
+      <c r="F2" s="158"/>
+      <c r="G2" s="158"/>
+      <c r="H2" s="158"/>
+      <c r="I2" s="158"/>
+      <c r="J2" s="158"/>
+      <c r="K2" s="158"/>
+      <c r="L2" s="158"/>
+      <c r="M2" s="158"/>
+      <c r="N2" s="158"/>
+      <c r="O2" s="158"/>
+      <c r="P2" s="158"/>
+      <c r="Q2" s="158"/>
+      <c r="R2" s="158"/>
+      <c r="S2" s="158"/>
+      <c r="T2" s="158"/>
+      <c r="U2" s="158"/>
+      <c r="V2" s="158"/>
+      <c r="W2" s="159"/>
       <c r="X2" s="82"/>
       <c r="Y2" s="82"/>
       <c r="Z2" s="82"/>
-    </row>
-    <row r="3" spans="1:28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AA2" s="82"/>
+    </row>
+    <row r="3" spans="1:29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="82"/>
       <c r="B3" s="83"/>
       <c r="C3" s="82"/>
@@ -4446,8 +4519,9 @@
       <c r="X3" s="82"/>
       <c r="Y3" s="82"/>
       <c r="Z3" s="82"/>
-    </row>
-    <row r="4" spans="1:28" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA3" s="82"/>
+    </row>
+    <row r="4" spans="1:29" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="82"/>
       <c r="B4" s="82"/>
       <c r="C4" s="82"/>
@@ -4465,22 +4539,23 @@
       <c r="O4" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="P4" s="157" t="str">
+      <c r="P4" s="160" t="str">
         <f>'Deelnemers en Scores'!H4</f>
         <v>yyyy-mm-dd</v>
       </c>
-      <c r="Q4" s="158"/>
-      <c r="R4" s="158"/>
-      <c r="S4" s="158"/>
-      <c r="T4" s="158"/>
-      <c r="U4" s="158"/>
+      <c r="Q4" s="161"/>
+      <c r="R4" s="161"/>
+      <c r="S4" s="161"/>
+      <c r="T4" s="161"/>
+      <c r="U4" s="161"/>
       <c r="V4" s="95"/>
       <c r="W4" s="96"/>
       <c r="X4" s="82"/>
       <c r="Y4" s="82"/>
       <c r="Z4" s="82"/>
-    </row>
-    <row r="5" spans="1:28" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA4" s="82"/>
+    </row>
+    <row r="5" spans="1:29" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="82"/>
       <c r="B5" s="83"/>
       <c r="C5" s="82"/>
@@ -4507,8 +4582,9 @@
       <c r="X5" s="82"/>
       <c r="Y5" s="82"/>
       <c r="Z5" s="82"/>
-    </row>
-    <row r="6" spans="1:28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AA5" s="82"/>
+    </row>
+    <row r="6" spans="1:29" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="82"/>
       <c r="B6" s="83"/>
       <c r="C6" s="82"/>
@@ -4535,48 +4611,52 @@
       <c r="X6" s="82"/>
       <c r="Y6" s="82"/>
       <c r="Z6" s="82"/>
-    </row>
-    <row r="7" spans="1:28" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA6" s="82"/>
+    </row>
+    <row r="7" spans="1:29" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="82"/>
       <c r="B7" s="97"/>
       <c r="C7" s="98"/>
       <c r="D7" s="99"/>
-      <c r="E7" s="152" t="s">
+      <c r="E7" s="155" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="159"/>
-      <c r="G7" s="159"/>
-      <c r="H7" s="159"/>
+      <c r="F7" s="162"/>
+      <c r="G7" s="162"/>
+      <c r="H7" s="162"/>
       <c r="I7" s="101"/>
-      <c r="J7" s="159" t="s">
+      <c r="J7" s="162" t="s">
         <v>36</v>
       </c>
-      <c r="K7" s="159"/>
-      <c r="L7" s="159"/>
-      <c r="M7" s="153"/>
+      <c r="K7" s="162"/>
+      <c r="L7" s="162"/>
+      <c r="M7" s="156"/>
       <c r="N7" s="100"/>
-      <c r="O7" s="152" t="s">
+      <c r="O7" s="155" t="s">
         <v>37</v>
       </c>
-      <c r="P7" s="159"/>
-      <c r="Q7" s="159"/>
-      <c r="R7" s="153"/>
+      <c r="P7" s="162"/>
+      <c r="Q7" s="162"/>
+      <c r="R7" s="156"/>
       <c r="S7" s="100" t="s">
-        <v>88</v>
-      </c>
-      <c r="T7" s="152" t="s">
         <v>87</v>
       </c>
-      <c r="U7" s="153"/>
+      <c r="T7" s="155" t="s">
+        <v>86</v>
+      </c>
+      <c r="U7" s="156"/>
       <c r="V7" s="101"/>
       <c r="W7" s="102" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="X7" s="82"/>
       <c r="Y7" s="82"/>
       <c r="Z7" s="82"/>
-    </row>
-    <row r="8" spans="1:28" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AA7" s="139" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="83"/>
       <c r="B8" s="103" t="s">
         <v>0</v>
@@ -4626,7 +4706,7 @@
         <v>4</v>
       </c>
       <c r="S8" s="110" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="T8" s="111" t="s">
         <v>49</v>
@@ -4639,8 +4719,11 @@
       <c r="X8" s="82"/>
       <c r="Y8" s="82"/>
       <c r="Z8" s="82"/>
-    </row>
-    <row r="9" spans="1:28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA8" s="140" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="83"/>
       <c r="B9" s="51">
         <f>IF('Deelnemers en Scores'!B9&gt;0,'Deelnemers en Scores'!B9,"")</f>
@@ -4718,66 +4801,70 @@
       </c>
       <c r="V9" s="88"/>
       <c r="W9" s="59">
-        <f>S9+D23</f>
+        <f t="shared" ref="W9:W20" si="7">S9+T9/10000+U9/10000000</f>
         <v>0</v>
       </c>
       <c r="X9" s="86"/>
       <c r="Y9" s="113" t="str">
-        <f>IF(W9&gt;0,IF(W9=W8,Y8,ROW()-ROW($Y$8)),"")</f>
-        <v/>
-      </c>
-      <c r="Z9" s="114" t="str">
-        <f>IF(Y9&lt;&gt;"","e","")</f>
-        <v/>
-      </c>
-      <c r="AA9" s="40"/>
+        <f t="shared" ref="Y9:Y20" si="8">IF(W9&gt;0,IF(W9=W8,Y8,ROW()-ROW($Y$8)),"")</f>
+        <v/>
+      </c>
+      <c r="Z9" s="138" t="str">
+        <f t="shared" ref="Z9:Z20" si="9">IF(Y9&lt;&gt;"",_xlfn.CONCAT(Y9,"e"),"")</f>
+        <v/>
+      </c>
+      <c r="AA9" s="137">
+        <f t="shared" ref="AA9:AA20" si="10">W9</f>
+        <v>0</v>
+      </c>
       <c r="AB9" s="40"/>
-    </row>
-    <row r="10" spans="1:28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AC9" s="40"/>
+    </row>
+    <row r="10" spans="1:29" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="83"/>
       <c r="B10" s="49">
-        <f>IF('Deelnemers en Scores'!B27&gt;0,'Deelnemers en Scores'!B27,"")</f>
-        <v>4</v>
+        <f>IF('Deelnemers en Scores'!B15&gt;0,'Deelnemers en Scores'!B15,"")</f>
+        <v>2</v>
       </c>
       <c r="C10" s="6" t="str">
-        <f>IF('Deelnemers en Scores'!F27="","",'Deelnemers en Scores'!F27)</f>
-        <v>Team naam 4</v>
+        <f>IF('Deelnemers en Scores'!F15="","",'Deelnemers en Scores'!F15)</f>
+        <v>Team naam 2</v>
       </c>
       <c r="D10" s="7" t="str">
-        <f>'Deelnemers en Scores'!D27</f>
-        <v>Vereniging 4</v>
+        <f>'Deelnemers en Scores'!D15</f>
+        <v>Vereniging 2</v>
       </c>
       <c r="E10" s="18" t="str">
-        <f>IF('Deelnemers en Scores'!H28=0,"",'Deelnemers en Scores'!H28)</f>
+        <f>IF('Deelnemers en Scores'!H16=0,"",'Deelnemers en Scores'!H16)</f>
         <v/>
       </c>
       <c r="F10" s="18" t="str">
-        <f>IF('Deelnemers en Scores'!H29=0,"",'Deelnemers en Scores'!H29)</f>
+        <f>IF('Deelnemers en Scores'!H17=0,"",'Deelnemers en Scores'!H17)</f>
         <v/>
       </c>
       <c r="G10" s="18" t="str">
-        <f>IF('Deelnemers en Scores'!H30=0,"",'Deelnemers en Scores'!H30)</f>
+        <f>IF('Deelnemers en Scores'!H18=0,"",'Deelnemers en Scores'!H18)</f>
         <v/>
       </c>
       <c r="H10" s="41" t="str">
-        <f>IF('Deelnemers en Scores'!H31=0,"",'Deelnemers en Scores'!H31)</f>
+        <f>IF('Deelnemers en Scores'!H19=0,"",'Deelnemers en Scores'!H19)</f>
         <v/>
       </c>
       <c r="I10" s="89"/>
       <c r="J10" s="18" t="str">
-        <f>IF('Deelnemers en Scores'!I28=0,"",'Deelnemers en Scores'!I28)</f>
+        <f>IF('Deelnemers en Scores'!I16=0,"",'Deelnemers en Scores'!I16)</f>
         <v/>
       </c>
       <c r="K10" s="18" t="str">
-        <f>IF('Deelnemers en Scores'!I29=0,"",'Deelnemers en Scores'!I29)</f>
+        <f>IF('Deelnemers en Scores'!I17=0,"",'Deelnemers en Scores'!I17)</f>
         <v/>
       </c>
       <c r="L10" s="18" t="str">
-        <f>IF('Deelnemers en Scores'!I30=0,"",'Deelnemers en Scores'!I30)</f>
+        <f>IF('Deelnemers en Scores'!I18=0,"",'Deelnemers en Scores'!I18)</f>
         <v/>
       </c>
       <c r="M10" s="41" t="str">
-        <f>IF('Deelnemers en Scores'!I31=0,"",'Deelnemers en Scores'!I31)</f>
+        <f>IF('Deelnemers en Scores'!I19=0,"",'Deelnemers en Scores'!I19)</f>
         <v/>
       </c>
       <c r="N10" s="89"/>
@@ -4811,64 +4898,68 @@
       </c>
       <c r="V10" s="89"/>
       <c r="W10" s="59">
-        <f t="shared" ref="W10:W20" si="7">S10+T10/10000+U10/10000000</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="X10" s="86"/>
       <c r="Y10" s="113" t="str">
-        <f t="shared" ref="Y10:Y20" si="8">IF(W10&gt;0,IF(W10=W9,Y9,ROW()-ROW($Y$8)),"")</f>
-        <v/>
-      </c>
-      <c r="Z10" s="114" t="str">
-        <f t="shared" ref="Z10:Z20" si="9">IF(Y10&lt;&gt;"","e","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="Z10" s="138" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AA10" s="137">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="83"/>
       <c r="B11" s="49">
-        <f>IF('Deelnemers en Scores'!B15&gt;0,'Deelnemers en Scores'!B15,"")</f>
-        <v>2</v>
+        <f>IF('Deelnemers en Scores'!B21&gt;0,'Deelnemers en Scores'!B21,"")</f>
+        <v>3</v>
       </c>
       <c r="C11" s="6" t="str">
-        <f>IF('Deelnemers en Scores'!F15="","",'Deelnemers en Scores'!F15)</f>
-        <v>Team naam 2</v>
+        <f>IF('Deelnemers en Scores'!F21="","",'Deelnemers en Scores'!F21)</f>
+        <v>Team naam 3</v>
       </c>
       <c r="D11" s="7" t="str">
-        <f>'Deelnemers en Scores'!D15</f>
-        <v>Vereniging 2</v>
+        <f>'Deelnemers en Scores'!D21</f>
+        <v>Vereniging 3</v>
       </c>
       <c r="E11" s="18" t="str">
-        <f>IF('Deelnemers en Scores'!H16=0,"",'Deelnemers en Scores'!H16)</f>
+        <f>IF('Deelnemers en Scores'!H22=0,"",'Deelnemers en Scores'!H22)</f>
         <v/>
       </c>
       <c r="F11" s="18" t="str">
-        <f>IF('Deelnemers en Scores'!H17=0,"",'Deelnemers en Scores'!H17)</f>
+        <f>IF('Deelnemers en Scores'!H23=0,"",'Deelnemers en Scores'!H23)</f>
         <v/>
       </c>
       <c r="G11" s="18" t="str">
-        <f>IF('Deelnemers en Scores'!H18=0,"",'Deelnemers en Scores'!H18)</f>
+        <f>IF('Deelnemers en Scores'!H24=0,"",'Deelnemers en Scores'!H24)</f>
         <v/>
       </c>
       <c r="H11" s="41" t="str">
-        <f>IF('Deelnemers en Scores'!H19=0,"",'Deelnemers en Scores'!H19)</f>
+        <f>IF('Deelnemers en Scores'!H25=0,"",'Deelnemers en Scores'!H25)</f>
         <v/>
       </c>
       <c r="I11" s="89"/>
       <c r="J11" s="18" t="str">
-        <f>IF('Deelnemers en Scores'!I16=0,"",'Deelnemers en Scores'!I16)</f>
+        <f>IF('Deelnemers en Scores'!I22=0,"",'Deelnemers en Scores'!I22)</f>
         <v/>
       </c>
       <c r="K11" s="18" t="str">
-        <f>IF('Deelnemers en Scores'!I17=0,"",'Deelnemers en Scores'!I17)</f>
+        <f>IF('Deelnemers en Scores'!I23=0,"",'Deelnemers en Scores'!I23)</f>
         <v/>
       </c>
       <c r="L11" s="18" t="str">
-        <f>IF('Deelnemers en Scores'!I18=0,"",'Deelnemers en Scores'!I18)</f>
+        <f>IF('Deelnemers en Scores'!I24=0,"",'Deelnemers en Scores'!I24)</f>
         <v/>
       </c>
       <c r="M11" s="41" t="str">
-        <f>IF('Deelnemers en Scores'!I19=0,"",'Deelnemers en Scores'!I19)</f>
+        <f>IF('Deelnemers en Scores'!I25=0,"",'Deelnemers en Scores'!I25)</f>
         <v/>
       </c>
       <c r="N11" s="89"/>
@@ -4910,56 +5001,60 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="Z11" s="114" t="str">
+      <c r="Z11" s="138" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-    </row>
-    <row r="12" spans="1:28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA11" s="137">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="83"/>
       <c r="B12" s="49">
-        <f>IF('Deelnemers en Scores'!B21&gt;0,'Deelnemers en Scores'!B21,"")</f>
-        <v>3</v>
+        <f>IF('Deelnemers en Scores'!B27&gt;0,'Deelnemers en Scores'!B27,"")</f>
+        <v>4</v>
       </c>
       <c r="C12" s="6" t="str">
-        <f>IF('Deelnemers en Scores'!F21="","",'Deelnemers en Scores'!F21)</f>
-        <v>Team naam 3</v>
+        <f>IF('Deelnemers en Scores'!F27="","",'Deelnemers en Scores'!F27)</f>
+        <v>Team naam 4</v>
       </c>
       <c r="D12" s="7" t="str">
-        <f>'Deelnemers en Scores'!D21</f>
-        <v>Vereniging 3</v>
+        <f>'Deelnemers en Scores'!D27</f>
+        <v>Vereniging 4</v>
       </c>
       <c r="E12" s="18" t="str">
-        <f>IF('Deelnemers en Scores'!H22=0,"",'Deelnemers en Scores'!H22)</f>
+        <f>IF('Deelnemers en Scores'!H28=0,"",'Deelnemers en Scores'!H28)</f>
         <v/>
       </c>
       <c r="F12" s="18" t="str">
-        <f>IF('Deelnemers en Scores'!H23=0,"",'Deelnemers en Scores'!H23)</f>
+        <f>IF('Deelnemers en Scores'!H29=0,"",'Deelnemers en Scores'!H29)</f>
         <v/>
       </c>
       <c r="G12" s="18" t="str">
-        <f>IF('Deelnemers en Scores'!H24=0,"",'Deelnemers en Scores'!H24)</f>
+        <f>IF('Deelnemers en Scores'!H30=0,"",'Deelnemers en Scores'!H30)</f>
         <v/>
       </c>
       <c r="H12" s="41" t="str">
-        <f>IF('Deelnemers en Scores'!H25=0,"",'Deelnemers en Scores'!H25)</f>
+        <f>IF('Deelnemers en Scores'!H31=0,"",'Deelnemers en Scores'!H31)</f>
         <v/>
       </c>
       <c r="I12" s="89"/>
       <c r="J12" s="18" t="str">
-        <f>IF('Deelnemers en Scores'!I22=0,"",'Deelnemers en Scores'!I22)</f>
+        <f>IF('Deelnemers en Scores'!I28=0,"",'Deelnemers en Scores'!I28)</f>
         <v/>
       </c>
       <c r="K12" s="18" t="str">
-        <f>IF('Deelnemers en Scores'!I23=0,"",'Deelnemers en Scores'!I23)</f>
+        <f>IF('Deelnemers en Scores'!I29=0,"",'Deelnemers en Scores'!I29)</f>
         <v/>
       </c>
       <c r="L12" s="18" t="str">
-        <f>IF('Deelnemers en Scores'!I24=0,"",'Deelnemers en Scores'!I24)</f>
+        <f>IF('Deelnemers en Scores'!I30=0,"",'Deelnemers en Scores'!I30)</f>
         <v/>
       </c>
       <c r="M12" s="41" t="str">
-        <f>IF('Deelnemers en Scores'!I25=0,"",'Deelnemers en Scores'!I25)</f>
+        <f>IF('Deelnemers en Scores'!I31=0,"",'Deelnemers en Scores'!I31)</f>
         <v/>
       </c>
       <c r="N12" s="89"/>
@@ -5001,12 +5096,16 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="Z12" s="114" t="str">
+      <c r="Z12" s="138" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-    </row>
-    <row r="13" spans="1:28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA12" s="137">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="83"/>
       <c r="B13" s="49">
         <f>IF('Deelnemers en Scores'!B33&gt;0,'Deelnemers en Scores'!B33,"")</f>
@@ -5092,12 +5191,16 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="Z13" s="114" t="str">
+      <c r="Z13" s="138" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-    </row>
-    <row r="14" spans="1:28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA13" s="137">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="83"/>
       <c r="B14" s="49">
         <f>IF('Deelnemers en Scores'!B39&gt;0,'Deelnemers en Scores'!B39,"")</f>
@@ -5183,12 +5286,16 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="Z14" s="114" t="str">
+      <c r="Z14" s="138" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-    </row>
-    <row r="15" spans="1:28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA14" s="137">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="83"/>
       <c r="B15" s="49">
         <f>IF('Deelnemers en Scores'!B45&gt;0,'Deelnemers en Scores'!B45,"")</f>
@@ -5274,12 +5381,16 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="Z15" s="114" t="str">
+      <c r="Z15" s="138" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-    </row>
-    <row r="16" spans="1:28" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA15" s="137">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="83"/>
       <c r="B16" s="49">
         <f>IF('Deelnemers en Scores'!B51&gt;0,'Deelnemers en Scores'!B51,"")</f>
@@ -5365,12 +5476,16 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="Z16" s="114" t="str">
+      <c r="Z16" s="138" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-    </row>
-    <row r="17" spans="1:26" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA16" s="137">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="83"/>
       <c r="B17" s="49">
         <f>IF('Deelnemers en Scores'!B57&gt;0,'Deelnemers en Scores'!B57,"")</f>
@@ -5456,12 +5571,16 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="Z17" s="114" t="str">
+      <c r="Z17" s="138" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-    </row>
-    <row r="18" spans="1:26" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA17" s="137">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="83"/>
       <c r="B18" s="49">
         <f>IF('Deelnemers en Scores'!B63&gt;0,'Deelnemers en Scores'!B63,"")</f>
@@ -5547,12 +5666,16 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="Z18" s="114" t="str">
+      <c r="Z18" s="138" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-    </row>
-    <row r="19" spans="1:26" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA18" s="137">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="83"/>
       <c r="B19" s="49">
         <f>IF('Deelnemers en Scores'!B69&gt;0,'Deelnemers en Scores'!B69,"")</f>
@@ -5638,12 +5761,16 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="Z19" s="114" t="str">
+      <c r="Z19" s="138" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-    </row>
-    <row r="20" spans="1:26" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AA19" s="137">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="83"/>
       <c r="B20" s="50">
         <f>IF('Deelnemers en Scores'!B75&gt;0,'Deelnemers en Scores'!B75,"")</f>
@@ -5729,12 +5856,16 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="Z20" s="114" t="str">
+      <c r="Z20" s="138" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-    </row>
-    <row r="21" spans="1:26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AA20" s="137">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="82"/>
       <c r="B21" s="84"/>
       <c r="C21" s="85"/>
@@ -5760,26 +5891,27 @@
       <c r="W21" s="85"/>
       <c r="X21" s="82"/>
       <c r="Y21" s="82"/>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="1:26" ht="80.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K23" s="151" t="s">
-        <v>84</v>
-      </c>
-      <c r="L23" s="151"/>
-      <c r="M23" s="151"/>
-      <c r="N23" s="151"/>
-      <c r="O23" s="151"/>
-      <c r="P23" s="151"/>
-      <c r="Q23" s="151"/>
-      <c r="R23" s="151"/>
-      <c r="S23" s="151"/>
-      <c r="T23" s="151"/>
-      <c r="U23" s="151"/>
-      <c r="V23" s="151"/>
-      <c r="W23" s="151"/>
-    </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Z21" s="82"/>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:27" ht="80.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K23" s="154" t="s">
+        <v>83</v>
+      </c>
+      <c r="L23" s="154"/>
+      <c r="M23" s="154"/>
+      <c r="N23" s="154"/>
+      <c r="O23" s="154"/>
+      <c r="P23" s="154"/>
+      <c r="Q23" s="154"/>
+      <c r="R23" s="154"/>
+      <c r="S23" s="154"/>
+      <c r="T23" s="154"/>
+      <c r="U23" s="154"/>
+      <c r="V23" s="154"/>
+      <c r="W23" s="154"/>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
       <c r="K24" s="87"/>
       <c r="L24" s="87"/>
       <c r="M24" s="87"/>
@@ -5796,7 +5928,11 @@
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <autoFilter ref="W8:W20" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
+  <autoFilter ref="B8:AA20" xr:uid="{00000000-0001-0000-0200-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B9:AA20">
+      <sortCondition ref="W8:W20"/>
+    </sortState>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B9:W20">
     <sortCondition descending="1" ref="W9"/>
   </sortState>
@@ -5810,6 +5946,11 @@
     <mergeCell ref="O7:R7"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
+  <conditionalFormatting sqref="AA9:AA20">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>INDEX(W9:W10,1)&lt;INDEX(W9:W10,2)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.19685039370078741" right="0.39370078740157483" top="0.78740157480314965" bottom="0.39370078740157483" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" scale="66" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0">

</xml_diff>